<commit_message>
fix: tambah formula dalam excel utk jumlah
</commit_message>
<xml_diff>
--- a/public/exports/BPE.xlsx
+++ b/public/exports/BPE.xlsx
@@ -8,14 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jiazh\gp2\public\exports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C78044A-6CA9-499E-A73C-9706373A6460}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36FC3E06-3AE9-4AC3-9B00-76762E44506C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BPE" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -622,7 +635,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -670,9 +683,6 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -697,128 +707,71 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -827,14 +780,71 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1159,44 +1169,44 @@
   </sheetPr>
   <dimension ref="A1:AP103"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30:AI30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9" style="2" customWidth="1"/>
-    <col min="2" max="2" width="13.81640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="11.26953125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="11.7265625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="4.54296875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="3.54296875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="13.77734375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="11.21875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="11.77734375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="4.5546875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="3.5546875" style="2" customWidth="1"/>
     <col min="7" max="7" width="4" style="2" customWidth="1"/>
-    <col min="8" max="8" width="3.7265625" style="2" customWidth="1"/>
-    <col min="9" max="9" width="4.7265625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="5.1796875" style="2" customWidth="1"/>
-    <col min="11" max="11" width="4.54296875" style="2" customWidth="1"/>
-    <col min="12" max="12" width="4.7265625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="3.77734375" style="2" customWidth="1"/>
+    <col min="9" max="9" width="4.77734375" style="2" customWidth="1"/>
+    <col min="10" max="10" width="5.21875" style="2" customWidth="1"/>
+    <col min="11" max="11" width="4.5546875" style="2" customWidth="1"/>
+    <col min="12" max="12" width="4.77734375" style="2" customWidth="1"/>
     <col min="13" max="13" width="7" style="2" customWidth="1"/>
-    <col min="14" max="14" width="6.54296875" style="2" customWidth="1"/>
-    <col min="15" max="15" width="10.1796875" style="2" customWidth="1"/>
-    <col min="16" max="16" width="11.26953125" style="2" customWidth="1"/>
-    <col min="17" max="17" width="8.7265625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="6.5546875" style="2" customWidth="1"/>
+    <col min="15" max="15" width="10.21875" style="2" customWidth="1"/>
+    <col min="16" max="16" width="11.21875" style="2" customWidth="1"/>
+    <col min="17" max="17" width="8.77734375" style="2" customWidth="1"/>
     <col min="18" max="18" width="8" style="2" customWidth="1"/>
-    <col min="19" max="22" width="4.54296875" style="2" customWidth="1"/>
+    <col min="19" max="22" width="4.5546875" style="2" customWidth="1"/>
     <col min="23" max="23" width="5" style="2" customWidth="1"/>
-    <col min="24" max="27" width="4.54296875" style="2" customWidth="1"/>
-    <col min="28" max="28" width="3.54296875" style="2" customWidth="1"/>
-    <col min="29" max="29" width="4.54296875" style="2" customWidth="1"/>
-    <col min="30" max="30" width="5.81640625" style="2" customWidth="1"/>
+    <col min="24" max="27" width="4.5546875" style="2" customWidth="1"/>
+    <col min="28" max="28" width="3.5546875" style="2" customWidth="1"/>
+    <col min="29" max="29" width="4.5546875" style="2" customWidth="1"/>
+    <col min="30" max="30" width="5.77734375" style="2" customWidth="1"/>
     <col min="31" max="31" width="6" style="2" customWidth="1"/>
-    <col min="32" max="32" width="4.453125" style="2" customWidth="1"/>
+    <col min="32" max="32" width="4.44140625" style="2" customWidth="1"/>
     <col min="33" max="33" width="5" style="2" customWidth="1"/>
     <col min="34" max="40" width="9" style="2" customWidth="1"/>
-    <col min="41" max="16384" width="14.453125" style="2"/>
+    <col min="41" max="16384" width="14.44140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:42" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -1238,7 +1248,7 @@
       <c r="AM1" s="1"/>
       <c r="AN1" s="1"/>
     </row>
-    <row r="2" spans="1:42" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:42" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1280,42 +1290,42 @@
       <c r="AM2" s="1"/>
       <c r="AN2" s="1"/>
     </row>
-    <row r="3" spans="1:42" ht="35.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:42" ht="35.700000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
-      <c r="C3" s="27"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
-      <c r="K3" s="25"/>
-      <c r="L3" s="25"/>
-      <c r="M3" s="25"/>
-      <c r="N3" s="25"/>
-      <c r="O3" s="25"/>
-      <c r="P3" s="25"/>
-      <c r="Q3" s="25"/>
-      <c r="R3" s="25"/>
-      <c r="S3" s="25"/>
-      <c r="T3" s="25"/>
-      <c r="U3" s="25"/>
-      <c r="V3" s="25"/>
-      <c r="W3" s="25"/>
-      <c r="X3" s="25"/>
-      <c r="Y3" s="25"/>
-      <c r="Z3" s="25"/>
-      <c r="AA3" s="25"/>
-      <c r="AB3" s="25"/>
-      <c r="AC3" s="25"/>
-      <c r="AD3" s="25"/>
-      <c r="AE3" s="25"/>
-      <c r="AF3" s="25"/>
-      <c r="AG3" s="24"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="24"/>
+      <c r="J3" s="24"/>
+      <c r="K3" s="24"/>
+      <c r="L3" s="24"/>
+      <c r="M3" s="24"/>
+      <c r="N3" s="24"/>
+      <c r="O3" s="24"/>
+      <c r="P3" s="24"/>
+      <c r="Q3" s="24"/>
+      <c r="R3" s="24"/>
+      <c r="S3" s="24"/>
+      <c r="T3" s="24"/>
+      <c r="U3" s="24"/>
+      <c r="V3" s="24"/>
+      <c r="W3" s="24"/>
+      <c r="X3" s="24"/>
+      <c r="Y3" s="24"/>
+      <c r="Z3" s="24"/>
+      <c r="AA3" s="24"/>
+      <c r="AB3" s="24"/>
+      <c r="AC3" s="24"/>
+      <c r="AD3" s="24"/>
+      <c r="AE3" s="24"/>
+      <c r="AF3" s="24"/>
+      <c r="AG3" s="23"/>
       <c r="AH3" s="1"/>
-      <c r="AI3" s="26" t="s">
+      <c r="AI3" s="25" t="s">
         <v>50</v>
       </c>
       <c r="AJ3" s="1"/>
@@ -1324,126 +1334,126 @@
       <c r="AM3" s="1"/>
       <c r="AN3" s="1"/>
     </row>
-    <row r="4" spans="1:42" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="22"/>
-      <c r="B4" s="22"/>
-      <c r="C4" s="23"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="24"/>
-      <c r="I4" s="24"/>
-      <c r="J4" s="24"/>
-      <c r="K4" s="24"/>
-      <c r="L4" s="24"/>
-      <c r="M4" s="24"/>
-      <c r="N4" s="24"/>
-      <c r="O4" s="24"/>
-      <c r="P4" s="24"/>
-      <c r="Q4" s="24"/>
-      <c r="R4" s="24"/>
-      <c r="S4" s="24"/>
-      <c r="T4" s="24"/>
-      <c r="U4" s="24"/>
-      <c r="V4" s="24"/>
-      <c r="W4" s="24"/>
-      <c r="X4" s="24"/>
-      <c r="Y4" s="24"/>
-      <c r="Z4" s="24"/>
-      <c r="AA4" s="24"/>
-      <c r="AB4" s="24"/>
-      <c r="AC4" s="24"/>
-      <c r="AD4" s="24"/>
-      <c r="AE4" s="24"/>
-      <c r="AF4" s="24"/>
-      <c r="AG4" s="24"/>
-      <c r="AH4" s="22"/>
-      <c r="AI4" s="22"/>
-      <c r="AJ4" s="22"/>
-      <c r="AK4" s="22"/>
-      <c r="AL4" s="22"/>
-      <c r="AM4" s="22"/>
-      <c r="AN4" s="22"/>
-    </row>
-    <row r="5" spans="1:42" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="22"/>
-      <c r="B5" s="22"/>
-      <c r="C5" s="23"/>
-      <c r="D5" s="24"/>
-      <c r="E5" s="24"/>
-      <c r="F5" s="24"/>
-      <c r="G5" s="24"/>
-      <c r="H5" s="24"/>
-      <c r="I5" s="24"/>
-      <c r="J5" s="24"/>
-      <c r="K5" s="24"/>
-      <c r="L5" s="24"/>
-      <c r="M5" s="24"/>
-      <c r="N5" s="24"/>
-      <c r="O5" s="24"/>
-      <c r="P5" s="24"/>
-      <c r="Q5" s="24"/>
-      <c r="R5" s="24"/>
-      <c r="S5" s="24"/>
-      <c r="T5" s="24"/>
-      <c r="U5" s="24"/>
-      <c r="V5" s="24"/>
-      <c r="W5" s="24"/>
-      <c r="X5" s="24"/>
-      <c r="Y5" s="24"/>
-      <c r="Z5" s="24"/>
-      <c r="AA5" s="24"/>
-      <c r="AB5" s="24"/>
-      <c r="AC5" s="24"/>
-      <c r="AD5" s="24"/>
-      <c r="AE5" s="24"/>
-      <c r="AF5" s="24"/>
-      <c r="AG5" s="24"/>
-      <c r="AH5" s="22"/>
-      <c r="AI5" s="22"/>
-      <c r="AJ5" s="22"/>
-      <c r="AK5" s="22"/>
-      <c r="AL5" s="22"/>
-      <c r="AM5" s="22"/>
-      <c r="AN5" s="22"/>
-    </row>
-    <row r="6" spans="1:42" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:42" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A4" s="21"/>
+      <c r="B4" s="21"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="23"/>
+      <c r="I4" s="23"/>
+      <c r="J4" s="23"/>
+      <c r="K4" s="23"/>
+      <c r="L4" s="23"/>
+      <c r="M4" s="23"/>
+      <c r="N4" s="23"/>
+      <c r="O4" s="23"/>
+      <c r="P4" s="23"/>
+      <c r="Q4" s="23"/>
+      <c r="R4" s="23"/>
+      <c r="S4" s="23"/>
+      <c r="T4" s="23"/>
+      <c r="U4" s="23"/>
+      <c r="V4" s="23"/>
+      <c r="W4" s="23"/>
+      <c r="X4" s="23"/>
+      <c r="Y4" s="23"/>
+      <c r="Z4" s="23"/>
+      <c r="AA4" s="23"/>
+      <c r="AB4" s="23"/>
+      <c r="AC4" s="23"/>
+      <c r="AD4" s="23"/>
+      <c r="AE4" s="23"/>
+      <c r="AF4" s="23"/>
+      <c r="AG4" s="23"/>
+      <c r="AH4" s="21"/>
+      <c r="AI4" s="21"/>
+      <c r="AJ4" s="21"/>
+      <c r="AK4" s="21"/>
+      <c r="AL4" s="21"/>
+      <c r="AM4" s="21"/>
+      <c r="AN4" s="21"/>
+    </row>
+    <row r="5" spans="1:42" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A5" s="21"/>
+      <c r="B5" s="21"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="23"/>
+      <c r="I5" s="23"/>
+      <c r="J5" s="23"/>
+      <c r="K5" s="23"/>
+      <c r="L5" s="23"/>
+      <c r="M5" s="23"/>
+      <c r="N5" s="23"/>
+      <c r="O5" s="23"/>
+      <c r="P5" s="23"/>
+      <c r="Q5" s="23"/>
+      <c r="R5" s="23"/>
+      <c r="S5" s="23"/>
+      <c r="T5" s="23"/>
+      <c r="U5" s="23"/>
+      <c r="V5" s="23"/>
+      <c r="W5" s="23"/>
+      <c r="X5" s="23"/>
+      <c r="Y5" s="23"/>
+      <c r="Z5" s="23"/>
+      <c r="AA5" s="23"/>
+      <c r="AB5" s="23"/>
+      <c r="AC5" s="23"/>
+      <c r="AD5" s="23"/>
+      <c r="AE5" s="23"/>
+      <c r="AF5" s="23"/>
+      <c r="AG5" s="23"/>
+      <c r="AH5" s="21"/>
+      <c r="AI5" s="21"/>
+      <c r="AJ5" s="21"/>
+      <c r="AK5" s="21"/>
+      <c r="AL5" s="21"/>
+      <c r="AM5" s="21"/>
+      <c r="AN5" s="21"/>
+    </row>
+    <row r="6" spans="1:42" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
-      <c r="C6" s="84" t="s">
+      <c r="C6" s="40" t="s">
         <v>47</v>
       </c>
-      <c r="D6" s="54"/>
-      <c r="E6" s="54"/>
-      <c r="F6" s="54"/>
-      <c r="G6" s="54"/>
-      <c r="H6" s="54"/>
-      <c r="I6" s="54"/>
-      <c r="J6" s="54"/>
-      <c r="K6" s="54"/>
-      <c r="L6" s="54"/>
-      <c r="M6" s="54"/>
-      <c r="N6" s="54"/>
-      <c r="O6" s="54"/>
-      <c r="P6" s="54"/>
-      <c r="Q6" s="54"/>
-      <c r="R6" s="54"/>
-      <c r="S6" s="54"/>
-      <c r="T6" s="54"/>
-      <c r="U6" s="54"/>
-      <c r="V6" s="54"/>
-      <c r="W6" s="54"/>
-      <c r="X6" s="54"/>
-      <c r="Y6" s="54"/>
-      <c r="Z6" s="54"/>
-      <c r="AA6" s="54"/>
-      <c r="AB6" s="54"/>
-      <c r="AC6" s="54"/>
-      <c r="AD6" s="54"/>
-      <c r="AE6" s="54"/>
-      <c r="AF6" s="54"/>
-      <c r="AG6" s="37"/>
+      <c r="D6" s="41"/>
+      <c r="E6" s="41"/>
+      <c r="F6" s="41"/>
+      <c r="G6" s="41"/>
+      <c r="H6" s="41"/>
+      <c r="I6" s="41"/>
+      <c r="J6" s="41"/>
+      <c r="K6" s="41"/>
+      <c r="L6" s="41"/>
+      <c r="M6" s="41"/>
+      <c r="N6" s="41"/>
+      <c r="O6" s="41"/>
+      <c r="P6" s="41"/>
+      <c r="Q6" s="41"/>
+      <c r="R6" s="41"/>
+      <c r="S6" s="41"/>
+      <c r="T6" s="41"/>
+      <c r="U6" s="41"/>
+      <c r="V6" s="41"/>
+      <c r="W6" s="41"/>
+      <c r="X6" s="41"/>
+      <c r="Y6" s="41"/>
+      <c r="Z6" s="41"/>
+      <c r="AA6" s="41"/>
+      <c r="AB6" s="41"/>
+      <c r="AC6" s="41"/>
+      <c r="AD6" s="41"/>
+      <c r="AE6" s="41"/>
+      <c r="AF6" s="41"/>
+      <c r="AG6" s="30"/>
       <c r="AH6" s="1"/>
       <c r="AI6" s="1"/>
       <c r="AJ6" s="1"/>
@@ -1452,7 +1462,7 @@
       <c r="AM6" s="1"/>
       <c r="AN6" s="1"/>
     </row>
-    <row r="7" spans="1:42" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:42" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="3"/>
@@ -1494,12 +1504,12 @@
       <c r="AM7" s="1"/>
       <c r="AN7" s="1"/>
     </row>
-    <row r="8" spans="1:42" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:42" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
-      <c r="B8" s="82" t="s">
+      <c r="B8" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="C8" s="37"/>
+      <c r="C8" s="30"/>
       <c r="D8" s="4"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
@@ -1538,12 +1548,12 @@
       <c r="AM8" s="1"/>
       <c r="AN8" s="1"/>
     </row>
-    <row r="9" spans="1:42" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:42" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
-      <c r="B9" s="82" t="s">
+      <c r="B9" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="37"/>
+      <c r="C9" s="30"/>
       <c r="D9" s="4"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
@@ -1582,7 +1592,7 @@
       <c r="AM9" s="1"/>
       <c r="AN9" s="1"/>
     </row>
-    <row r="10" spans="1:42" ht="9" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:42" ht="9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="4"/>
@@ -1624,62 +1634,62 @@
       <c r="AM10" s="1"/>
       <c r="AN10" s="1"/>
     </row>
-    <row r="11" spans="1:42" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:42" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
-      <c r="B11" s="65" t="s">
+      <c r="B11" s="53" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="79" t="s">
+      <c r="C11" s="59" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="38" t="s">
+      <c r="D11" s="72" t="s">
         <v>35</v>
       </c>
-      <c r="E11" s="42" t="s">
+      <c r="E11" s="46" t="s">
         <v>52</v>
       </c>
-      <c r="F11" s="43"/>
-      <c r="G11" s="44"/>
-      <c r="H11" s="83" t="s">
-        <v>0</v>
-      </c>
-      <c r="I11" s="70"/>
-      <c r="J11" s="71"/>
-      <c r="K11" s="68" t="s">
+      <c r="F11" s="76"/>
+      <c r="G11" s="77"/>
+      <c r="H11" s="34" t="s">
+        <v>0</v>
+      </c>
+      <c r="I11" s="35"/>
+      <c r="J11" s="36"/>
+      <c r="K11" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="L11" s="58"/>
-      <c r="M11" s="58"/>
-      <c r="N11" s="58"/>
-      <c r="O11" s="58"/>
-      <c r="P11" s="58"/>
-      <c r="Q11" s="58"/>
-      <c r="R11" s="66"/>
-      <c r="S11" s="69" t="s">
+      <c r="L11" s="43"/>
+      <c r="M11" s="43"/>
+      <c r="N11" s="43"/>
+      <c r="O11" s="43"/>
+      <c r="P11" s="43"/>
+      <c r="Q11" s="43"/>
+      <c r="R11" s="56"/>
+      <c r="S11" s="58" t="s">
         <v>2</v>
       </c>
-      <c r="T11" s="58"/>
-      <c r="U11" s="58"/>
-      <c r="V11" s="58"/>
-      <c r="W11" s="58"/>
-      <c r="X11" s="58"/>
-      <c r="Y11" s="58"/>
-      <c r="Z11" s="58"/>
-      <c r="AA11" s="58"/>
-      <c r="AB11" s="58"/>
-      <c r="AC11" s="35"/>
-      <c r="AD11" s="42" t="s">
+      <c r="T11" s="43"/>
+      <c r="U11" s="43"/>
+      <c r="V11" s="43"/>
+      <c r="W11" s="43"/>
+      <c r="X11" s="43"/>
+      <c r="Y11" s="43"/>
+      <c r="Z11" s="43"/>
+      <c r="AA11" s="43"/>
+      <c r="AB11" s="43"/>
+      <c r="AC11" s="44"/>
+      <c r="AD11" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="AE11" s="70"/>
-      <c r="AF11" s="71"/>
-      <c r="AG11" s="55" t="s">
+      <c r="AE11" s="35"/>
+      <c r="AF11" s="36"/>
+      <c r="AG11" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="AH11" s="55" t="s">
+      <c r="AH11" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="AI11" s="55" t="s">
+      <c r="AI11" s="45" t="s">
         <v>46</v>
       </c>
       <c r="AJ11" s="6"/>
@@ -1690,50 +1700,50 @@
       <c r="AO11" s="6"/>
       <c r="AP11" s="6"/>
     </row>
-    <row r="12" spans="1:42" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:42" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
-      <c r="B12" s="56"/>
-      <c r="C12" s="80"/>
-      <c r="D12" s="39"/>
-      <c r="E12" s="45"/>
-      <c r="F12" s="46"/>
-      <c r="G12" s="47"/>
-      <c r="H12" s="72"/>
-      <c r="I12" s="73"/>
-      <c r="J12" s="74"/>
-      <c r="K12" s="57" t="s">
+      <c r="B12" s="32"/>
+      <c r="C12" s="60"/>
+      <c r="D12" s="73"/>
+      <c r="E12" s="78"/>
+      <c r="F12" s="79"/>
+      <c r="G12" s="80"/>
+      <c r="H12" s="37"/>
+      <c r="I12" s="38"/>
+      <c r="J12" s="39"/>
+      <c r="K12" s="55" t="s">
         <v>9</v>
       </c>
-      <c r="L12" s="58"/>
-      <c r="M12" s="58"/>
-      <c r="N12" s="58"/>
-      <c r="O12" s="58"/>
-      <c r="P12" s="58"/>
-      <c r="Q12" s="58"/>
-      <c r="R12" s="66"/>
-      <c r="S12" s="67" t="s">
+      <c r="L12" s="43"/>
+      <c r="M12" s="43"/>
+      <c r="N12" s="43"/>
+      <c r="O12" s="43"/>
+      <c r="P12" s="43"/>
+      <c r="Q12" s="43"/>
+      <c r="R12" s="56"/>
+      <c r="S12" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="T12" s="58"/>
-      <c r="U12" s="35"/>
-      <c r="V12" s="67" t="s">
+      <c r="T12" s="43"/>
+      <c r="U12" s="44"/>
+      <c r="V12" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="W12" s="58"/>
-      <c r="X12" s="58"/>
-      <c r="Y12" s="58"/>
-      <c r="Z12" s="58"/>
-      <c r="AA12" s="58"/>
-      <c r="AB12" s="35"/>
-      <c r="AC12" s="53" t="s">
+      <c r="W12" s="43"/>
+      <c r="X12" s="43"/>
+      <c r="Y12" s="43"/>
+      <c r="Z12" s="43"/>
+      <c r="AA12" s="43"/>
+      <c r="AB12" s="44"/>
+      <c r="AC12" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="AD12" s="72"/>
-      <c r="AE12" s="73"/>
-      <c r="AF12" s="74"/>
-      <c r="AG12" s="56"/>
-      <c r="AH12" s="56"/>
-      <c r="AI12" s="56"/>
+      <c r="AD12" s="37"/>
+      <c r="AE12" s="38"/>
+      <c r="AF12" s="39"/>
+      <c r="AG12" s="32"/>
+      <c r="AH12" s="32"/>
+      <c r="AI12" s="32"/>
       <c r="AJ12" s="7"/>
       <c r="AK12" s="7"/>
       <c r="AL12" s="7"/>
@@ -1742,78 +1752,78 @@
       <c r="AO12" s="7"/>
       <c r="AP12" s="7"/>
     </row>
-    <row r="13" spans="1:42" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:42" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
-      <c r="B13" s="56"/>
-      <c r="C13" s="80"/>
-      <c r="D13" s="40"/>
-      <c r="E13" s="52" t="s">
+      <c r="B13" s="32"/>
+      <c r="C13" s="60"/>
+      <c r="D13" s="74"/>
+      <c r="E13" s="83" t="s">
         <v>22</v>
       </c>
-      <c r="F13" s="52"/>
-      <c r="G13" s="76" t="s">
+      <c r="F13" s="83"/>
+      <c r="G13" s="48" t="s">
         <v>49</v>
       </c>
-      <c r="H13" s="77" t="s">
+      <c r="H13" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="I13" s="53" t="s">
+      <c r="I13" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="J13" s="53" t="s">
+      <c r="J13" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="K13" s="57" t="s">
+      <c r="K13" s="55" t="s">
         <v>12</v>
       </c>
-      <c r="L13" s="58"/>
-      <c r="M13" s="58"/>
-      <c r="N13" s="58"/>
-      <c r="O13" s="58"/>
-      <c r="P13" s="58"/>
-      <c r="Q13" s="58"/>
-      <c r="R13" s="35"/>
-      <c r="S13" s="55" t="s">
+      <c r="L13" s="43"/>
+      <c r="M13" s="43"/>
+      <c r="N13" s="43"/>
+      <c r="O13" s="43"/>
+      <c r="P13" s="43"/>
+      <c r="Q13" s="43"/>
+      <c r="R13" s="44"/>
+      <c r="S13" s="45" t="s">
         <v>13</v>
       </c>
-      <c r="T13" s="55" t="s">
+      <c r="T13" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="U13" s="53" t="s">
+      <c r="U13" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="V13" s="75" t="s">
+      <c r="V13" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="W13" s="55" t="s">
+      <c r="W13" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="X13" s="53" t="s">
+      <c r="X13" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="Y13" s="53" t="s">
+      <c r="Y13" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="Z13" s="53" t="s">
+      <c r="Z13" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="AA13" s="53" t="s">
+      <c r="AA13" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="AB13" s="53" t="s">
+      <c r="AB13" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="AC13" s="56"/>
-      <c r="AD13" s="59" t="s">
+      <c r="AC13" s="32"/>
+      <c r="AD13" s="63" t="s">
         <v>36</v>
       </c>
-      <c r="AE13" s="34" t="s">
+      <c r="AE13" s="71" t="s">
         <v>23</v>
       </c>
-      <c r="AF13" s="35"/>
-      <c r="AG13" s="56"/>
-      <c r="AH13" s="56"/>
-      <c r="AI13" s="56"/>
+      <c r="AF13" s="44"/>
+      <c r="AG13" s="32"/>
+      <c r="AH13" s="32"/>
+      <c r="AI13" s="32"/>
       <c r="AJ13" s="6"/>
       <c r="AK13" s="6"/>
       <c r="AL13" s="6"/>
@@ -1822,60 +1832,60 @@
       <c r="AO13" s="6"/>
       <c r="AP13" s="7"/>
     </row>
-    <row r="14" spans="1:42" ht="68.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:42" ht="68.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
-      <c r="B14" s="56"/>
-      <c r="C14" s="80"/>
-      <c r="D14" s="40"/>
-      <c r="E14" s="50" t="s">
+      <c r="B14" s="32"/>
+      <c r="C14" s="60"/>
+      <c r="D14" s="74"/>
+      <c r="E14" s="49" t="s">
         <v>51</v>
       </c>
-      <c r="F14" s="48" t="s">
+      <c r="F14" s="81" t="s">
         <v>8</v>
       </c>
-      <c r="G14" s="50"/>
-      <c r="H14" s="78"/>
-      <c r="I14" s="56"/>
-      <c r="J14" s="56"/>
-      <c r="K14" s="53" t="s">
+      <c r="G14" s="49"/>
+      <c r="H14" s="52"/>
+      <c r="I14" s="32"/>
+      <c r="J14" s="32"/>
+      <c r="K14" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="L14" s="62" t="s">
+      <c r="L14" s="54" t="s">
         <v>25</v>
       </c>
-      <c r="M14" s="58"/>
-      <c r="N14" s="35"/>
-      <c r="O14" s="62" t="s">
+      <c r="M14" s="43"/>
+      <c r="N14" s="44"/>
+      <c r="O14" s="54" t="s">
         <v>37</v>
       </c>
-      <c r="P14" s="35"/>
-      <c r="Q14" s="28" t="s">
+      <c r="P14" s="44"/>
+      <c r="Q14" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="R14" s="28" t="s">
+      <c r="R14" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="S14" s="56"/>
-      <c r="T14" s="56"/>
-      <c r="U14" s="56"/>
-      <c r="V14" s="56"/>
-      <c r="W14" s="56"/>
-      <c r="X14" s="56"/>
-      <c r="Y14" s="56"/>
-      <c r="Z14" s="56"/>
-      <c r="AA14" s="56"/>
-      <c r="AB14" s="56"/>
-      <c r="AC14" s="56"/>
-      <c r="AD14" s="60"/>
-      <c r="AE14" s="53" t="s">
+      <c r="S14" s="32"/>
+      <c r="T14" s="32"/>
+      <c r="U14" s="32"/>
+      <c r="V14" s="32"/>
+      <c r="W14" s="32"/>
+      <c r="X14" s="32"/>
+      <c r="Y14" s="32"/>
+      <c r="Z14" s="32"/>
+      <c r="AA14" s="32"/>
+      <c r="AB14" s="32"/>
+      <c r="AC14" s="32"/>
+      <c r="AD14" s="64"/>
+      <c r="AE14" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="AF14" s="53" t="s">
+      <c r="AF14" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="AG14" s="56"/>
-      <c r="AH14" s="56"/>
-      <c r="AI14" s="56"/>
+      <c r="AG14" s="32"/>
+      <c r="AH14" s="32"/>
+      <c r="AI14" s="32"/>
       <c r="AJ14" s="6"/>
       <c r="AK14" s="6"/>
       <c r="AL14" s="6"/>
@@ -1884,18 +1894,18 @@
       <c r="AO14" s="6"/>
       <c r="AP14" s="7"/>
     </row>
-    <row r="15" spans="1:42" ht="52.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:42" ht="52.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
-      <c r="B15" s="31"/>
-      <c r="C15" s="81"/>
-      <c r="D15" s="41"/>
-      <c r="E15" s="51"/>
-      <c r="F15" s="49"/>
-      <c r="G15" s="51"/>
-      <c r="H15" s="74"/>
-      <c r="I15" s="31"/>
-      <c r="J15" s="31"/>
-      <c r="K15" s="31"/>
+      <c r="B15" s="33"/>
+      <c r="C15" s="61"/>
+      <c r="D15" s="75"/>
+      <c r="E15" s="50"/>
+      <c r="F15" s="82"/>
+      <c r="G15" s="50"/>
+      <c r="H15" s="39"/>
+      <c r="I15" s="33"/>
+      <c r="J15" s="33"/>
+      <c r="K15" s="33"/>
       <c r="L15" s="8">
         <v>0</v>
       </c>
@@ -1914,26 +1924,26 @@
       <c r="Q15" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="R15" s="29" t="s">
+      <c r="R15" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="S15" s="31"/>
-      <c r="T15" s="31"/>
-      <c r="U15" s="31"/>
-      <c r="V15" s="31"/>
-      <c r="W15" s="31"/>
-      <c r="X15" s="31"/>
-      <c r="Y15" s="31"/>
-      <c r="Z15" s="31"/>
-      <c r="AA15" s="31"/>
-      <c r="AB15" s="31"/>
-      <c r="AC15" s="31"/>
-      <c r="AD15" s="61"/>
-      <c r="AE15" s="31"/>
-      <c r="AF15" s="31"/>
-      <c r="AG15" s="31"/>
-      <c r="AH15" s="31"/>
-      <c r="AI15" s="31"/>
+      <c r="S15" s="33"/>
+      <c r="T15" s="33"/>
+      <c r="U15" s="33"/>
+      <c r="V15" s="33"/>
+      <c r="W15" s="33"/>
+      <c r="X15" s="33"/>
+      <c r="Y15" s="33"/>
+      <c r="Z15" s="33"/>
+      <c r="AA15" s="33"/>
+      <c r="AB15" s="33"/>
+      <c r="AC15" s="33"/>
+      <c r="AD15" s="65"/>
+      <c r="AE15" s="33"/>
+      <c r="AF15" s="33"/>
+      <c r="AG15" s="33"/>
+      <c r="AH15" s="33"/>
+      <c r="AI15" s="33"/>
       <c r="AJ15" s="6"/>
       <c r="AK15" s="6"/>
       <c r="AL15" s="6"/>
@@ -1942,7 +1952,7 @@
       <c r="AO15" s="6"/>
       <c r="AP15" s="7"/>
     </row>
-    <row r="16" spans="1:42" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:42" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
       <c r="B16" s="9">
         <v>3</v>
@@ -2054,9 +2064,9 @@
       <c r="AO16" s="7"/>
       <c r="AP16" s="7"/>
     </row>
-    <row r="17" spans="1:42" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:42" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
-      <c r="B17" s="32" t="s">
+      <c r="B17" s="69" t="s">
         <v>48</v>
       </c>
       <c r="C17" s="13" t="s">
@@ -2102,9 +2112,9 @@
       <c r="AO17" s="7"/>
       <c r="AP17" s="7"/>
     </row>
-    <row r="18" spans="1:42" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:42" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
-      <c r="B18" s="33"/>
+      <c r="B18" s="70"/>
       <c r="C18" s="13" t="s">
         <v>40</v>
       </c>
@@ -2148,9 +2158,9 @@
       <c r="AO18" s="7"/>
       <c r="AP18" s="7"/>
     </row>
-    <row r="19" spans="1:42" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:42" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
-      <c r="B19" s="30" t="s">
+      <c r="B19" s="68" t="s">
         <v>38</v>
       </c>
       <c r="C19" s="13" t="s">
@@ -2196,9 +2206,9 @@
       <c r="AO19" s="7"/>
       <c r="AP19" s="7"/>
     </row>
-    <row r="20" spans="1:42" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:42" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
-      <c r="B20" s="31"/>
+      <c r="B20" s="33"/>
       <c r="C20" s="13" t="s">
         <v>40</v>
       </c>
@@ -2242,9 +2252,9 @@
       <c r="AO20" s="1"/>
       <c r="AP20" s="1"/>
     </row>
-    <row r="21" spans="1:42" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:42" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
-      <c r="B21" s="30" t="s">
+      <c r="B21" s="68" t="s">
         <v>41</v>
       </c>
       <c r="C21" s="13" t="s">
@@ -2290,9 +2300,9 @@
       <c r="AO21" s="1"/>
       <c r="AP21" s="1"/>
     </row>
-    <row r="22" spans="1:42" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:42" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
-      <c r="B22" s="31"/>
+      <c r="B22" s="33"/>
       <c r="C22" s="13" t="s">
         <v>40</v>
       </c>
@@ -2336,9 +2346,9 @@
       <c r="AO22" s="1"/>
       <c r="AP22" s="1"/>
     </row>
-    <row r="23" spans="1:42" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:42" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
-      <c r="B23" s="30" t="s">
+      <c r="B23" s="68" t="s">
         <v>42</v>
       </c>
       <c r="C23" s="13" t="s">
@@ -2384,9 +2394,9 @@
       <c r="AO23" s="1"/>
       <c r="AP23" s="1"/>
     </row>
-    <row r="24" spans="1:42" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:42" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
-      <c r="B24" s="31"/>
+      <c r="B24" s="33"/>
       <c r="C24" s="13" t="s">
         <v>40</v>
       </c>
@@ -2430,9 +2440,9 @@
       <c r="AO24" s="1"/>
       <c r="AP24" s="1"/>
     </row>
-    <row r="25" spans="1:42" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:42" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
-      <c r="B25" s="30" t="s">
+      <c r="B25" s="68" t="s">
         <v>43</v>
       </c>
       <c r="C25" s="13" t="s">
@@ -2478,9 +2488,9 @@
       <c r="AO25" s="1"/>
       <c r="AP25" s="1"/>
     </row>
-    <row r="26" spans="1:42" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:42" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1"/>
-      <c r="B26" s="31"/>
+      <c r="B26" s="33"/>
       <c r="C26" s="13" t="s">
         <v>40</v>
       </c>
@@ -2524,9 +2534,9 @@
       <c r="AO26" s="1"/>
       <c r="AP26" s="1"/>
     </row>
-    <row r="27" spans="1:42" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:42" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1"/>
-      <c r="B27" s="63" t="s">
+      <c r="B27" s="66" t="s">
         <v>44</v>
       </c>
       <c r="C27" s="13" t="s">
@@ -2572,9 +2582,9 @@
       <c r="AO27" s="1"/>
       <c r="AP27" s="1"/>
     </row>
-    <row r="28" spans="1:42" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:42" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1"/>
-      <c r="B28" s="64"/>
+      <c r="B28" s="67"/>
       <c r="C28" s="13" t="s">
         <v>40</v>
       </c>
@@ -2618,46 +2628,142 @@
       <c r="AO28" s="1"/>
       <c r="AP28" s="1"/>
     </row>
-    <row r="29" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1"/>
-      <c r="B29" s="65" t="s">
+      <c r="B29" s="53" t="s">
         <v>30</v>
       </c>
       <c r="C29" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="D29" s="13"/>
-      <c r="E29" s="13"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="15"/>
-      <c r="H29" s="16"/>
-      <c r="I29" s="16"/>
-      <c r="J29" s="16"/>
-      <c r="K29" s="15"/>
-      <c r="L29" s="15"/>
-      <c r="M29" s="15"/>
-      <c r="N29" s="15"/>
-      <c r="O29" s="15"/>
-      <c r="P29" s="15"/>
-      <c r="Q29" s="15"/>
-      <c r="R29" s="15"/>
-      <c r="S29" s="17"/>
-      <c r="T29" s="17"/>
-      <c r="U29" s="17"/>
-      <c r="V29" s="17"/>
-      <c r="W29" s="17"/>
-      <c r="X29" s="17"/>
-      <c r="Y29" s="17"/>
-      <c r="Z29" s="17"/>
-      <c r="AA29" s="17"/>
-      <c r="AB29" s="17"/>
-      <c r="AC29" s="17"/>
-      <c r="AD29" s="17"/>
-      <c r="AE29" s="17"/>
-      <c r="AF29" s="17"/>
-      <c r="AG29" s="17"/>
-      <c r="AH29" s="17"/>
-      <c r="AI29" s="15"/>
+      <c r="D29" s="13">
+        <f>SUM(D17,D19,D21,D23,D25,D27)</f>
+        <v>0</v>
+      </c>
+      <c r="E29" s="13">
+        <f t="shared" ref="E29:AI29" si="0">SUM(E17,E19,E21,E23,E25,E27)</f>
+        <v>0</v>
+      </c>
+      <c r="F29" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G29" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H29" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I29" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J29" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K29" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L29" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M29" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N29" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O29" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P29" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q29" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R29" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="S29" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="T29" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="U29" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="V29" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="W29" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="X29" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Y29" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Z29" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AA29" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AB29" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AC29" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AD29" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AE29" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AF29" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AG29" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AH29" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AI29" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="AJ29" s="1"/>
       <c r="AK29" s="1"/>
       <c r="AL29" s="1"/>
@@ -2666,44 +2772,140 @@
       <c r="AO29" s="1"/>
       <c r="AP29" s="1"/>
     </row>
-    <row r="30" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1"/>
-      <c r="B30" s="31"/>
+      <c r="B30" s="33"/>
       <c r="C30" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="8"/>
-      <c r="H30" s="19"/>
-      <c r="I30" s="19"/>
-      <c r="J30" s="19"/>
-      <c r="K30" s="18"/>
-      <c r="L30" s="18"/>
-      <c r="M30" s="18"/>
-      <c r="N30" s="18"/>
-      <c r="O30" s="18"/>
-      <c r="P30" s="18"/>
-      <c r="Q30" s="18"/>
-      <c r="R30" s="18"/>
-      <c r="S30" s="18"/>
-      <c r="T30" s="18"/>
-      <c r="U30" s="18"/>
-      <c r="V30" s="18"/>
-      <c r="W30" s="18"/>
-      <c r="X30" s="18"/>
-      <c r="Y30" s="18"/>
-      <c r="Z30" s="18"/>
-      <c r="AA30" s="18"/>
-      <c r="AB30" s="18"/>
-      <c r="AC30" s="18"/>
-      <c r="AD30" s="18"/>
-      <c r="AE30" s="18"/>
-      <c r="AF30" s="18"/>
-      <c r="AG30" s="18"/>
-      <c r="AH30" s="18"/>
-      <c r="AI30" s="18"/>
+      <c r="D30" s="13">
+        <f>SUM(D18,D20,D22,D24,D26,D28)</f>
+        <v>0</v>
+      </c>
+      <c r="E30" s="13">
+        <f t="shared" ref="E30:AI30" si="1">SUM(E18,E20,E22,E24,E26,E28)</f>
+        <v>0</v>
+      </c>
+      <c r="F30" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G30" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H30" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I30" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J30" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K30" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L30" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M30" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N30" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O30" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P30" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q30" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R30" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="S30" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="T30" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="U30" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="V30" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="W30" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="X30" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Y30" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Z30" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AA30" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AB30" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AC30" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AD30" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AE30" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AF30" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AG30" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AH30" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AI30" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="AJ30" s="1"/>
       <c r="AK30" s="1"/>
       <c r="AL30" s="1"/>
@@ -2712,7 +2914,7 @@
       <c r="AO30" s="1"/>
       <c r="AP30" s="1"/>
     </row>
-    <row r="31" spans="1:42" ht="13.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:42" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -2754,25 +2956,25 @@
       <c r="AM31" s="1"/>
       <c r="AN31" s="1"/>
     </row>
-    <row r="32" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1"/>
-      <c r="B32" s="36" t="s">
+      <c r="B32" s="62" t="s">
         <v>31</v>
       </c>
-      <c r="C32" s="37"/>
-      <c r="D32" s="20"/>
-      <c r="E32" s="20"/>
-      <c r="F32" s="20"/>
-      <c r="G32" s="20"/>
-      <c r="H32" s="20"/>
-      <c r="I32" s="20"/>
-      <c r="J32" s="20"/>
-      <c r="K32" s="20"/>
-      <c r="L32" s="20"/>
-      <c r="M32" s="20"/>
-      <c r="N32" s="20"/>
-      <c r="O32" s="20"/>
-      <c r="P32" s="20"/>
+      <c r="C32" s="30"/>
+      <c r="D32" s="19"/>
+      <c r="E32" s="19"/>
+      <c r="F32" s="19"/>
+      <c r="G32" s="19"/>
+      <c r="H32" s="19"/>
+      <c r="I32" s="19"/>
+      <c r="J32" s="19"/>
+      <c r="K32" s="19"/>
+      <c r="L32" s="19"/>
+      <c r="M32" s="19"/>
+      <c r="N32" s="19"/>
+      <c r="O32" s="19"/>
+      <c r="P32" s="19"/>
       <c r="Q32" s="1"/>
       <c r="R32" s="1"/>
       <c r="S32" s="1"/>
@@ -2798,25 +3000,25 @@
       <c r="AM32" s="1"/>
       <c r="AN32" s="1"/>
     </row>
-    <row r="33" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="1"/>
-      <c r="B33" s="36" t="s">
+      <c r="B33" s="62" t="s">
         <v>45</v>
       </c>
-      <c r="C33" s="54"/>
-      <c r="D33" s="54"/>
-      <c r="E33" s="37"/>
-      <c r="F33" s="20"/>
-      <c r="G33" s="20"/>
-      <c r="H33" s="20"/>
-      <c r="I33" s="20"/>
-      <c r="J33" s="20"/>
-      <c r="K33" s="20"/>
-      <c r="L33" s="20"/>
-      <c r="M33" s="20"/>
-      <c r="N33" s="20"/>
-      <c r="O33" s="20"/>
-      <c r="P33" s="20"/>
+      <c r="C33" s="41"/>
+      <c r="D33" s="41"/>
+      <c r="E33" s="30"/>
+      <c r="F33" s="19"/>
+      <c r="G33" s="19"/>
+      <c r="H33" s="19"/>
+      <c r="I33" s="19"/>
+      <c r="J33" s="19"/>
+      <c r="K33" s="19"/>
+      <c r="L33" s="19"/>
+      <c r="M33" s="19"/>
+      <c r="N33" s="19"/>
+      <c r="O33" s="19"/>
+      <c r="P33" s="19"/>
       <c r="Q33" s="1"/>
       <c r="R33" s="1"/>
       <c r="S33" s="1"/>
@@ -2842,23 +3044,23 @@
       <c r="AM33" s="1"/>
       <c r="AN33" s="1"/>
     </row>
-    <row r="34" spans="1:40" ht="4.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:40" ht="4.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
-      <c r="C34" s="21"/>
-      <c r="D34" s="21"/>
-      <c r="E34" s="20"/>
-      <c r="F34" s="20"/>
-      <c r="G34" s="20"/>
-      <c r="H34" s="20"/>
-      <c r="I34" s="20"/>
-      <c r="J34" s="20"/>
-      <c r="K34" s="20"/>
-      <c r="L34" s="20"/>
-      <c r="M34" s="20"/>
-      <c r="N34" s="20"/>
-      <c r="O34" s="20"/>
-      <c r="P34" s="20"/>
+      <c r="C34" s="20"/>
+      <c r="D34" s="20"/>
+      <c r="E34" s="19"/>
+      <c r="F34" s="19"/>
+      <c r="G34" s="19"/>
+      <c r="H34" s="19"/>
+      <c r="I34" s="19"/>
+      <c r="J34" s="19"/>
+      <c r="K34" s="19"/>
+      <c r="L34" s="19"/>
+      <c r="M34" s="19"/>
+      <c r="N34" s="19"/>
+      <c r="O34" s="19"/>
+      <c r="P34" s="19"/>
       <c r="Q34" s="1"/>
       <c r="R34" s="1"/>
       <c r="S34" s="1"/>
@@ -2884,7 +3086,7 @@
       <c r="AM34" s="1"/>
       <c r="AN34" s="1"/>
     </row>
-    <row r="35" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -2926,7 +3128,7 @@
       <c r="AM35" s="1"/>
       <c r="AN35" s="1"/>
     </row>
-    <row r="36" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -2968,7 +3170,7 @@
       <c r="AM36" s="1"/>
       <c r="AN36" s="1"/>
     </row>
-    <row r="37" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -3010,7 +3212,7 @@
       <c r="AM37" s="1"/>
       <c r="AN37" s="1"/>
     </row>
-    <row r="38" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -3052,7 +3254,7 @@
       <c r="AM38" s="1"/>
       <c r="AN38" s="1"/>
     </row>
-    <row r="39" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -3094,7 +3296,7 @@
       <c r="AM39" s="1"/>
       <c r="AN39" s="1"/>
     </row>
-    <row r="40" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -3136,7 +3338,7 @@
       <c r="AM40" s="1"/>
       <c r="AN40" s="1"/>
     </row>
-    <row r="41" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -3178,7 +3380,7 @@
       <c r="AM41" s="1"/>
       <c r="AN41" s="1"/>
     </row>
-    <row r="42" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -3220,7 +3422,7 @@
       <c r="AM42" s="1"/>
       <c r="AN42" s="1"/>
     </row>
-    <row r="43" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -3262,7 +3464,7 @@
       <c r="AM43" s="1"/>
       <c r="AN43" s="1"/>
     </row>
-    <row r="44" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -3304,7 +3506,7 @@
       <c r="AM44" s="1"/>
       <c r="AN44" s="1"/>
     </row>
-    <row r="45" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -3346,7 +3548,7 @@
       <c r="AM45" s="1"/>
       <c r="AN45" s="1"/>
     </row>
-    <row r="46" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
@@ -3388,7 +3590,7 @@
       <c r="AM46" s="1"/>
       <c r="AN46" s="1"/>
     </row>
-    <row r="47" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -3430,7 +3632,7 @@
       <c r="AM47" s="1"/>
       <c r="AN47" s="1"/>
     </row>
-    <row r="48" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -3472,7 +3674,7 @@
       <c r="AM48" s="1"/>
       <c r="AN48" s="1"/>
     </row>
-    <row r="49" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -3514,7 +3716,7 @@
       <c r="AM49" s="1"/>
       <c r="AN49" s="1"/>
     </row>
-    <row r="50" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -3556,7 +3758,7 @@
       <c r="AM50" s="1"/>
       <c r="AN50" s="1"/>
     </row>
-    <row r="51" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -3598,7 +3800,7 @@
       <c r="AM51" s="1"/>
       <c r="AN51" s="1"/>
     </row>
-    <row r="52" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -3640,7 +3842,7 @@
       <c r="AM52" s="1"/>
       <c r="AN52" s="1"/>
     </row>
-    <row r="53" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -3682,7 +3884,7 @@
       <c r="AM53" s="1"/>
       <c r="AN53" s="1"/>
     </row>
-    <row r="54" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
@@ -3724,7 +3926,7 @@
       <c r="AM54" s="1"/>
       <c r="AN54" s="1"/>
     </row>
-    <row r="55" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
@@ -3766,7 +3968,7 @@
       <c r="AM55" s="1"/>
       <c r="AN55" s="1"/>
     </row>
-    <row r="56" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
@@ -3808,7 +4010,7 @@
       <c r="AM56" s="1"/>
       <c r="AN56" s="1"/>
     </row>
-    <row r="57" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
@@ -3850,7 +4052,7 @@
       <c r="AM57" s="1"/>
       <c r="AN57" s="1"/>
     </row>
-    <row r="58" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -3892,7 +4094,7 @@
       <c r="AM58" s="1"/>
       <c r="AN58" s="1"/>
     </row>
-    <row r="59" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
@@ -3934,7 +4136,7 @@
       <c r="AM59" s="1"/>
       <c r="AN59" s="1"/>
     </row>
-    <row r="60" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -3976,7 +4178,7 @@
       <c r="AM60" s="1"/>
       <c r="AN60" s="1"/>
     </row>
-    <row r="61" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
@@ -4018,7 +4220,7 @@
       <c r="AM61" s="1"/>
       <c r="AN61" s="1"/>
     </row>
-    <row r="62" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
@@ -4060,7 +4262,7 @@
       <c r="AM62" s="1"/>
       <c r="AN62" s="1"/>
     </row>
-    <row r="63" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
@@ -4102,7 +4304,7 @@
       <c r="AM63" s="1"/>
       <c r="AN63" s="1"/>
     </row>
-    <row r="64" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
@@ -4144,7 +4346,7 @@
       <c r="AM64" s="1"/>
       <c r="AN64" s="1"/>
     </row>
-    <row r="65" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
@@ -4186,7 +4388,7 @@
       <c r="AM65" s="1"/>
       <c r="AN65" s="1"/>
     </row>
-    <row r="66" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
@@ -4228,7 +4430,7 @@
       <c r="AM66" s="1"/>
       <c r="AN66" s="1"/>
     </row>
-    <row r="67" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
@@ -4270,7 +4472,7 @@
       <c r="AM67" s="1"/>
       <c r="AN67" s="1"/>
     </row>
-    <row r="68" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
@@ -4312,7 +4514,7 @@
       <c r="AM68" s="1"/>
       <c r="AN68" s="1"/>
     </row>
-    <row r="69" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
@@ -4354,7 +4556,7 @@
       <c r="AM69" s="1"/>
       <c r="AN69" s="1"/>
     </row>
-    <row r="70" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="1"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
@@ -4396,7 +4598,7 @@
       <c r="AM70" s="1"/>
       <c r="AN70" s="1"/>
     </row>
-    <row r="71" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="1"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
@@ -4438,7 +4640,7 @@
       <c r="AM71" s="1"/>
       <c r="AN71" s="1"/>
     </row>
-    <row r="72" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="1"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
@@ -4480,7 +4682,7 @@
       <c r="AM72" s="1"/>
       <c r="AN72" s="1"/>
     </row>
-    <row r="73" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
@@ -4522,7 +4724,7 @@
       <c r="AM73" s="1"/>
       <c r="AN73" s="1"/>
     </row>
-    <row r="74" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
@@ -4564,7 +4766,7 @@
       <c r="AM74" s="1"/>
       <c r="AN74" s="1"/>
     </row>
-    <row r="75" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="1"/>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
@@ -4606,7 +4808,7 @@
       <c r="AM75" s="1"/>
       <c r="AN75" s="1"/>
     </row>
-    <row r="76" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="1"/>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
@@ -4648,7 +4850,7 @@
       <c r="AM76" s="1"/>
       <c r="AN76" s="1"/>
     </row>
-    <row r="77" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
@@ -4690,7 +4892,7 @@
       <c r="AM77" s="1"/>
       <c r="AN77" s="1"/>
     </row>
-    <row r="78" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
@@ -4732,7 +4934,7 @@
       <c r="AM78" s="1"/>
       <c r="AN78" s="1"/>
     </row>
-    <row r="79" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
@@ -4774,7 +4976,7 @@
       <c r="AM79" s="1"/>
       <c r="AN79" s="1"/>
     </row>
-    <row r="80" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
@@ -4816,7 +5018,7 @@
       <c r="AM80" s="1"/>
       <c r="AN80" s="1"/>
     </row>
-    <row r="81" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" s="1"/>
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
@@ -4858,7 +5060,7 @@
       <c r="AM81" s="1"/>
       <c r="AN81" s="1"/>
     </row>
-    <row r="82" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
@@ -4900,7 +5102,7 @@
       <c r="AM82" s="1"/>
       <c r="AN82" s="1"/>
     </row>
-    <row r="83" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83" s="1"/>
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
@@ -4942,7 +5144,7 @@
       <c r="AM83" s="1"/>
       <c r="AN83" s="1"/>
     </row>
-    <row r="84" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84" s="1"/>
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
@@ -4984,7 +5186,7 @@
       <c r="AM84" s="1"/>
       <c r="AN84" s="1"/>
     </row>
-    <row r="85" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" s="1"/>
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
@@ -5026,7 +5228,7 @@
       <c r="AM85" s="1"/>
       <c r="AN85" s="1"/>
     </row>
-    <row r="86" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86" s="1"/>
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
@@ -5068,7 +5270,7 @@
       <c r="AM86" s="1"/>
       <c r="AN86" s="1"/>
     </row>
-    <row r="87" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" s="1"/>
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
@@ -5110,7 +5312,7 @@
       <c r="AM87" s="1"/>
       <c r="AN87" s="1"/>
     </row>
-    <row r="88" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88" s="1"/>
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
@@ -5152,7 +5354,7 @@
       <c r="AM88" s="1"/>
       <c r="AN88" s="1"/>
     </row>
-    <row r="89" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" s="1"/>
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
@@ -5194,7 +5396,7 @@
       <c r="AM89" s="1"/>
       <c r="AN89" s="1"/>
     </row>
-    <row r="90" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90" s="1"/>
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
@@ -5236,7 +5438,7 @@
       <c r="AM90" s="1"/>
       <c r="AN90" s="1"/>
     </row>
-    <row r="91" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A91" s="1"/>
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
@@ -5278,7 +5480,7 @@
       <c r="AM91" s="1"/>
       <c r="AN91" s="1"/>
     </row>
-    <row r="92" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A92" s="1"/>
       <c r="B92" s="1"/>
       <c r="C92" s="1"/>
@@ -5320,7 +5522,7 @@
       <c r="AM92" s="1"/>
       <c r="AN92" s="1"/>
     </row>
-    <row r="93" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A93" s="1"/>
       <c r="B93" s="1"/>
       <c r="C93" s="1"/>
@@ -5362,7 +5564,7 @@
       <c r="AM93" s="1"/>
       <c r="AN93" s="1"/>
     </row>
-    <row r="94" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A94" s="1"/>
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
@@ -5404,7 +5606,7 @@
       <c r="AM94" s="1"/>
       <c r="AN94" s="1"/>
     </row>
-    <row r="95" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A95" s="1"/>
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
@@ -5446,7 +5648,7 @@
       <c r="AM95" s="1"/>
       <c r="AN95" s="1"/>
     </row>
-    <row r="96" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A96" s="1"/>
       <c r="B96" s="1"/>
       <c r="C96" s="1"/>
@@ -5488,7 +5690,7 @@
       <c r="AM96" s="1"/>
       <c r="AN96" s="1"/>
     </row>
-    <row r="97" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A97" s="1"/>
       <c r="B97" s="1"/>
       <c r="C97" s="1"/>
@@ -5530,7 +5732,7 @@
       <c r="AM97" s="1"/>
       <c r="AN97" s="1"/>
     </row>
-    <row r="98" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A98" s="1"/>
       <c r="B98" s="1"/>
       <c r="C98" s="1"/>
@@ -5572,7 +5774,7 @@
       <c r="AM98" s="1"/>
       <c r="AN98" s="1"/>
     </row>
-    <row r="99" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A99" s="1"/>
       <c r="B99" s="1"/>
       <c r="C99" s="1"/>
@@ -5614,7 +5816,7 @@
       <c r="AM99" s="1"/>
       <c r="AN99" s="1"/>
     </row>
-    <row r="100" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A100" s="1"/>
       <c r="B100" s="1"/>
       <c r="C100" s="1"/>
@@ -5656,7 +5858,7 @@
       <c r="AM100" s="1"/>
       <c r="AN100" s="1"/>
     </row>
-    <row r="101" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A101" s="1"/>
       <c r="B101" s="1"/>
       <c r="C101" s="1"/>
@@ -5698,7 +5900,7 @@
       <c r="AM101" s="1"/>
       <c r="AN101" s="1"/>
     </row>
-    <row r="102" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B102" s="1"/>
       <c r="C102" s="1"/>
       <c r="D102" s="1"/>
@@ -5732,7 +5934,7 @@
       <c r="AF102" s="1"/>
       <c r="AG102" s="1"/>
     </row>
-    <row r="103" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B103" s="1"/>
       <c r="C103" s="1"/>
       <c r="D103" s="1"/>
@@ -5768,32 +5970,16 @@
     </row>
   </sheetData>
   <mergeCells count="52">
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="I13:I15"/>
-    <mergeCell ref="J13:J15"/>
-    <mergeCell ref="H11:J12"/>
-    <mergeCell ref="C6:AG6"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="S12:U12"/>
-    <mergeCell ref="AI11:AI15"/>
-    <mergeCell ref="AD11:AF12"/>
-    <mergeCell ref="U13:U15"/>
-    <mergeCell ref="V13:V15"/>
-    <mergeCell ref="G13:G15"/>
-    <mergeCell ref="H13:H15"/>
-    <mergeCell ref="AH11:AH15"/>
-    <mergeCell ref="AF14:AF15"/>
-    <mergeCell ref="B11:B15"/>
-    <mergeCell ref="L14:N14"/>
-    <mergeCell ref="X13:X15"/>
-    <mergeCell ref="Y13:Y15"/>
-    <mergeCell ref="K12:R12"/>
-    <mergeCell ref="V12:AB12"/>
-    <mergeCell ref="AC12:AC15"/>
-    <mergeCell ref="K11:R11"/>
-    <mergeCell ref="S11:AC11"/>
-    <mergeCell ref="AG11:AG15"/>
-    <mergeCell ref="C11:C15"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="AE13:AF13"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="D11:D15"/>
+    <mergeCell ref="E11:G12"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="AE14:AE15"/>
     <mergeCell ref="B33:E33"/>
     <mergeCell ref="S13:S15"/>
     <mergeCell ref="K13:R13"/>
@@ -5810,16 +5996,32 @@
     <mergeCell ref="B29:B30"/>
     <mergeCell ref="K14:K15"/>
     <mergeCell ref="B19:B20"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="AE13:AF13"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="D11:D15"/>
-    <mergeCell ref="E11:G12"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="AE14:AE15"/>
+    <mergeCell ref="AI11:AI15"/>
+    <mergeCell ref="AD11:AF12"/>
+    <mergeCell ref="U13:U15"/>
+    <mergeCell ref="V13:V15"/>
+    <mergeCell ref="G13:G15"/>
+    <mergeCell ref="H13:H15"/>
+    <mergeCell ref="AH11:AH15"/>
+    <mergeCell ref="AF14:AF15"/>
+    <mergeCell ref="L14:N14"/>
+    <mergeCell ref="X13:X15"/>
+    <mergeCell ref="Y13:Y15"/>
+    <mergeCell ref="K12:R12"/>
+    <mergeCell ref="V12:AB12"/>
+    <mergeCell ref="AC12:AC15"/>
+    <mergeCell ref="K11:R11"/>
+    <mergeCell ref="S11:AC11"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="I13:I15"/>
+    <mergeCell ref="J13:J15"/>
+    <mergeCell ref="H11:J12"/>
+    <mergeCell ref="C6:AG6"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="S12:U12"/>
+    <mergeCell ref="B11:B15"/>
+    <mergeCell ref="AG11:AG15"/>
+    <mergeCell ref="C11:C15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" scale="49" fitToHeight="0" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
fix: upload bpe dan 201 baru
</commit_message>
<xml_diff>
--- a/public/exports/BPE.xlsx
+++ b/public/exports/BPE.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jiazh\gp2\public\exports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\calypso\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36FC3E06-3AE9-4AC3-9B00-76762E44506C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C79A648-3E1F-4A80-B29E-F11AD97399B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-1185" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BPE" sheetId="2" r:id="rId1"/>
@@ -635,7 +635,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -663,25 +663,11 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -707,16 +693,100 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -724,53 +794,35 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -780,71 +832,29 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1170,43 +1180,43 @@
   <dimension ref="A1:AP103"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30:AI30"/>
+      <selection activeCell="D17" sqref="D17:AI30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" style="2" customWidth="1"/>
-    <col min="2" max="2" width="13.77734375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="11.21875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="11.77734375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="4.5546875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="3.5546875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="4.5703125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="3.5703125" style="2" customWidth="1"/>
     <col min="7" max="7" width="4" style="2" customWidth="1"/>
-    <col min="8" max="8" width="3.77734375" style="2" customWidth="1"/>
-    <col min="9" max="9" width="4.77734375" style="2" customWidth="1"/>
-    <col min="10" max="10" width="5.21875" style="2" customWidth="1"/>
-    <col min="11" max="11" width="4.5546875" style="2" customWidth="1"/>
-    <col min="12" max="12" width="4.77734375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="3.7109375" style="2" customWidth="1"/>
+    <col min="9" max="9" width="4.7109375" style="2" customWidth="1"/>
+    <col min="10" max="10" width="5.28515625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="4.5703125" style="2" customWidth="1"/>
+    <col min="12" max="12" width="4.7109375" style="2" customWidth="1"/>
     <col min="13" max="13" width="7" style="2" customWidth="1"/>
-    <col min="14" max="14" width="6.5546875" style="2" customWidth="1"/>
-    <col min="15" max="15" width="10.21875" style="2" customWidth="1"/>
-    <col min="16" max="16" width="11.21875" style="2" customWidth="1"/>
-    <col min="17" max="17" width="8.77734375" style="2" customWidth="1"/>
+    <col min="14" max="14" width="6.5703125" style="2" customWidth="1"/>
+    <col min="15" max="15" width="10.28515625" style="2" customWidth="1"/>
+    <col min="16" max="16" width="11.28515625" style="2" customWidth="1"/>
+    <col min="17" max="17" width="8.7109375" style="2" customWidth="1"/>
     <col min="18" max="18" width="8" style="2" customWidth="1"/>
-    <col min="19" max="22" width="4.5546875" style="2" customWidth="1"/>
+    <col min="19" max="22" width="4.5703125" style="2" customWidth="1"/>
     <col min="23" max="23" width="5" style="2" customWidth="1"/>
-    <col min="24" max="27" width="4.5546875" style="2" customWidth="1"/>
-    <col min="28" max="28" width="3.5546875" style="2" customWidth="1"/>
-    <col min="29" max="29" width="4.5546875" style="2" customWidth="1"/>
-    <col min="30" max="30" width="5.77734375" style="2" customWidth="1"/>
+    <col min="24" max="27" width="4.5703125" style="2" customWidth="1"/>
+    <col min="28" max="28" width="3.5703125" style="2" customWidth="1"/>
+    <col min="29" max="29" width="4.5703125" style="2" customWidth="1"/>
+    <col min="30" max="30" width="5.7109375" style="2" customWidth="1"/>
     <col min="31" max="31" width="6" style="2" customWidth="1"/>
-    <col min="32" max="32" width="4.44140625" style="2" customWidth="1"/>
+    <col min="32" max="32" width="4.42578125" style="2" customWidth="1"/>
     <col min="33" max="33" width="5" style="2" customWidth="1"/>
     <col min="34" max="40" width="9" style="2" customWidth="1"/>
-    <col min="41" max="16384" width="14.44140625" style="2"/>
+    <col min="41" max="16384" width="14.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:42" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -1248,7 +1258,7 @@
       <c r="AM1" s="1"/>
       <c r="AN1" s="1"/>
     </row>
-    <row r="2" spans="1:42" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:42" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1290,42 +1300,42 @@
       <c r="AM2" s="1"/>
       <c r="AN2" s="1"/>
     </row>
-    <row r="3" spans="1:42" ht="35.700000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:42" ht="35.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="24"/>
-      <c r="I3" s="24"/>
-      <c r="J3" s="24"/>
-      <c r="K3" s="24"/>
-      <c r="L3" s="24"/>
-      <c r="M3" s="24"/>
-      <c r="N3" s="24"/>
-      <c r="O3" s="24"/>
-      <c r="P3" s="24"/>
-      <c r="Q3" s="24"/>
-      <c r="R3" s="24"/>
-      <c r="S3" s="24"/>
-      <c r="T3" s="24"/>
-      <c r="U3" s="24"/>
-      <c r="V3" s="24"/>
-      <c r="W3" s="24"/>
-      <c r="X3" s="24"/>
-      <c r="Y3" s="24"/>
-      <c r="Z3" s="24"/>
-      <c r="AA3" s="24"/>
-      <c r="AB3" s="24"/>
-      <c r="AC3" s="24"/>
-      <c r="AD3" s="24"/>
-      <c r="AE3" s="24"/>
-      <c r="AF3" s="24"/>
-      <c r="AG3" s="23"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="18"/>
+      <c r="L3" s="18"/>
+      <c r="M3" s="18"/>
+      <c r="N3" s="18"/>
+      <c r="O3" s="18"/>
+      <c r="P3" s="18"/>
+      <c r="Q3" s="18"/>
+      <c r="R3" s="18"/>
+      <c r="S3" s="18"/>
+      <c r="T3" s="18"/>
+      <c r="U3" s="18"/>
+      <c r="V3" s="18"/>
+      <c r="W3" s="18"/>
+      <c r="X3" s="18"/>
+      <c r="Y3" s="18"/>
+      <c r="Z3" s="18"/>
+      <c r="AA3" s="18"/>
+      <c r="AB3" s="18"/>
+      <c r="AC3" s="18"/>
+      <c r="AD3" s="18"/>
+      <c r="AE3" s="18"/>
+      <c r="AF3" s="18"/>
+      <c r="AG3" s="17"/>
       <c r="AH3" s="1"/>
-      <c r="AI3" s="25" t="s">
+      <c r="AI3" s="19" t="s">
         <v>50</v>
       </c>
       <c r="AJ3" s="1"/>
@@ -1334,125 +1344,125 @@
       <c r="AM3" s="1"/>
       <c r="AN3" s="1"/>
     </row>
-    <row r="4" spans="1:42" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A4" s="21"/>
-      <c r="B4" s="21"/>
-      <c r="C4" s="22"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="23"/>
-      <c r="F4" s="23"/>
-      <c r="G4" s="23"/>
-      <c r="H4" s="23"/>
-      <c r="I4" s="23"/>
-      <c r="J4" s="23"/>
-      <c r="K4" s="23"/>
-      <c r="L4" s="23"/>
-      <c r="M4" s="23"/>
-      <c r="N4" s="23"/>
-      <c r="O4" s="23"/>
-      <c r="P4" s="23"/>
-      <c r="Q4" s="23"/>
-      <c r="R4" s="23"/>
-      <c r="S4" s="23"/>
-      <c r="T4" s="23"/>
-      <c r="U4" s="23"/>
-      <c r="V4" s="23"/>
-      <c r="W4" s="23"/>
-      <c r="X4" s="23"/>
-      <c r="Y4" s="23"/>
-      <c r="Z4" s="23"/>
-      <c r="AA4" s="23"/>
-      <c r="AB4" s="23"/>
-      <c r="AC4" s="23"/>
-      <c r="AD4" s="23"/>
-      <c r="AE4" s="23"/>
-      <c r="AF4" s="23"/>
-      <c r="AG4" s="23"/>
-      <c r="AH4" s="21"/>
-      <c r="AI4" s="21"/>
-      <c r="AJ4" s="21"/>
-      <c r="AK4" s="21"/>
-      <c r="AL4" s="21"/>
-      <c r="AM4" s="21"/>
-      <c r="AN4" s="21"/>
-    </row>
-    <row r="5" spans="1:42" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A5" s="21"/>
-      <c r="B5" s="21"/>
-      <c r="C5" s="22"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="23"/>
-      <c r="G5" s="23"/>
-      <c r="H5" s="23"/>
-      <c r="I5" s="23"/>
-      <c r="J5" s="23"/>
-      <c r="K5" s="23"/>
-      <c r="L5" s="23"/>
-      <c r="M5" s="23"/>
-      <c r="N5" s="23"/>
-      <c r="O5" s="23"/>
-      <c r="P5" s="23"/>
-      <c r="Q5" s="23"/>
-      <c r="R5" s="23"/>
-      <c r="S5" s="23"/>
-      <c r="T5" s="23"/>
-      <c r="U5" s="23"/>
-      <c r="V5" s="23"/>
-      <c r="W5" s="23"/>
-      <c r="X5" s="23"/>
-      <c r="Y5" s="23"/>
-      <c r="Z5" s="23"/>
-      <c r="AA5" s="23"/>
-      <c r="AB5" s="23"/>
-      <c r="AC5" s="23"/>
-      <c r="AD5" s="23"/>
-      <c r="AE5" s="23"/>
-      <c r="AF5" s="23"/>
-      <c r="AG5" s="23"/>
-      <c r="AH5" s="21"/>
-      <c r="AI5" s="21"/>
-      <c r="AJ5" s="21"/>
-      <c r="AK5" s="21"/>
-      <c r="AL5" s="21"/>
-      <c r="AM5" s="21"/>
-      <c r="AN5" s="21"/>
-    </row>
-    <row r="6" spans="1:42" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A4" s="15"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="17"/>
+      <c r="K4" s="17"/>
+      <c r="L4" s="17"/>
+      <c r="M4" s="17"/>
+      <c r="N4" s="17"/>
+      <c r="O4" s="17"/>
+      <c r="P4" s="17"/>
+      <c r="Q4" s="17"/>
+      <c r="R4" s="17"/>
+      <c r="S4" s="17"/>
+      <c r="T4" s="17"/>
+      <c r="U4" s="17"/>
+      <c r="V4" s="17"/>
+      <c r="W4" s="17"/>
+      <c r="X4" s="17"/>
+      <c r="Y4" s="17"/>
+      <c r="Z4" s="17"/>
+      <c r="AA4" s="17"/>
+      <c r="AB4" s="17"/>
+      <c r="AC4" s="17"/>
+      <c r="AD4" s="17"/>
+      <c r="AE4" s="17"/>
+      <c r="AF4" s="17"/>
+      <c r="AG4" s="17"/>
+      <c r="AH4" s="15"/>
+      <c r="AI4" s="15"/>
+      <c r="AJ4" s="15"/>
+      <c r="AK4" s="15"/>
+      <c r="AL4" s="15"/>
+      <c r="AM4" s="15"/>
+      <c r="AN4" s="15"/>
+    </row>
+    <row r="5" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A5" s="15"/>
+      <c r="B5" s="15"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="17"/>
+      <c r="K5" s="17"/>
+      <c r="L5" s="17"/>
+      <c r="M5" s="17"/>
+      <c r="N5" s="17"/>
+      <c r="O5" s="17"/>
+      <c r="P5" s="17"/>
+      <c r="Q5" s="17"/>
+      <c r="R5" s="17"/>
+      <c r="S5" s="17"/>
+      <c r="T5" s="17"/>
+      <c r="U5" s="17"/>
+      <c r="V5" s="17"/>
+      <c r="W5" s="17"/>
+      <c r="X5" s="17"/>
+      <c r="Y5" s="17"/>
+      <c r="Z5" s="17"/>
+      <c r="AA5" s="17"/>
+      <c r="AB5" s="17"/>
+      <c r="AC5" s="17"/>
+      <c r="AD5" s="17"/>
+      <c r="AE5" s="17"/>
+      <c r="AF5" s="17"/>
+      <c r="AG5" s="17"/>
+      <c r="AH5" s="15"/>
+      <c r="AI5" s="15"/>
+      <c r="AJ5" s="15"/>
+      <c r="AK5" s="15"/>
+      <c r="AL5" s="15"/>
+      <c r="AM5" s="15"/>
+      <c r="AN5" s="15"/>
+    </row>
+    <row r="6" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
-      <c r="C6" s="40" t="s">
+      <c r="C6" s="74" t="s">
         <v>47</v>
       </c>
-      <c r="D6" s="41"/>
-      <c r="E6" s="41"/>
-      <c r="F6" s="41"/>
-      <c r="G6" s="41"/>
-      <c r="H6" s="41"/>
-      <c r="I6" s="41"/>
-      <c r="J6" s="41"/>
-      <c r="K6" s="41"/>
-      <c r="L6" s="41"/>
-      <c r="M6" s="41"/>
-      <c r="N6" s="41"/>
-      <c r="O6" s="41"/>
-      <c r="P6" s="41"/>
-      <c r="Q6" s="41"/>
-      <c r="R6" s="41"/>
-      <c r="S6" s="41"/>
-      <c r="T6" s="41"/>
-      <c r="U6" s="41"/>
-      <c r="V6" s="41"/>
-      <c r="W6" s="41"/>
-      <c r="X6" s="41"/>
-      <c r="Y6" s="41"/>
-      <c r="Z6" s="41"/>
-      <c r="AA6" s="41"/>
-      <c r="AB6" s="41"/>
-      <c r="AC6" s="41"/>
-      <c r="AD6" s="41"/>
-      <c r="AE6" s="41"/>
-      <c r="AF6" s="41"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="47"/>
+      <c r="G6" s="47"/>
+      <c r="H6" s="47"/>
+      <c r="I6" s="47"/>
+      <c r="J6" s="47"/>
+      <c r="K6" s="47"/>
+      <c r="L6" s="47"/>
+      <c r="M6" s="47"/>
+      <c r="N6" s="47"/>
+      <c r="O6" s="47"/>
+      <c r="P6" s="47"/>
+      <c r="Q6" s="47"/>
+      <c r="R6" s="47"/>
+      <c r="S6" s="47"/>
+      <c r="T6" s="47"/>
+      <c r="U6" s="47"/>
+      <c r="V6" s="47"/>
+      <c r="W6" s="47"/>
+      <c r="X6" s="47"/>
+      <c r="Y6" s="47"/>
+      <c r="Z6" s="47"/>
+      <c r="AA6" s="47"/>
+      <c r="AB6" s="47"/>
+      <c r="AC6" s="47"/>
+      <c r="AD6" s="47"/>
+      <c r="AE6" s="47"/>
+      <c r="AF6" s="47"/>
       <c r="AG6" s="30"/>
       <c r="AH6" s="1"/>
       <c r="AI6" s="1"/>
@@ -1462,7 +1472,7 @@
       <c r="AM6" s="1"/>
       <c r="AN6" s="1"/>
     </row>
-    <row r="7" spans="1:42" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="3"/>
@@ -1504,9 +1514,9 @@
       <c r="AM7" s="1"/>
       <c r="AN7" s="1"/>
     </row>
-    <row r="8" spans="1:42" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:42" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
-      <c r="B8" s="29" t="s">
+      <c r="B8" s="72" t="s">
         <v>53</v>
       </c>
       <c r="C8" s="30"/>
@@ -1548,9 +1558,9 @@
       <c r="AM8" s="1"/>
       <c r="AN8" s="1"/>
     </row>
-    <row r="9" spans="1:42" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:42" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
-      <c r="B9" s="29" t="s">
+      <c r="B9" s="72" t="s">
         <v>32</v>
       </c>
       <c r="C9" s="30"/>
@@ -1592,7 +1602,7 @@
       <c r="AM9" s="1"/>
       <c r="AN9" s="1"/>
     </row>
-    <row r="10" spans="1:42" ht="9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:42" ht="9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="4"/>
@@ -1634,62 +1644,62 @@
       <c r="AM10" s="1"/>
       <c r="AN10" s="1"/>
     </row>
-    <row r="11" spans="1:42" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:42" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
-      <c r="B11" s="53" t="s">
+      <c r="B11" s="58" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="59" t="s">
+      <c r="C11" s="75" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="72" t="s">
+      <c r="D11" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="E11" s="46" t="s">
+      <c r="E11" s="35" t="s">
         <v>52</v>
       </c>
-      <c r="F11" s="76"/>
-      <c r="G11" s="77"/>
-      <c r="H11" s="34" t="s">
-        <v>0</v>
-      </c>
-      <c r="I11" s="35"/>
-      <c r="J11" s="36"/>
-      <c r="K11" s="57" t="s">
+      <c r="F11" s="36"/>
+      <c r="G11" s="37"/>
+      <c r="H11" s="73" t="s">
+        <v>0</v>
+      </c>
+      <c r="I11" s="59"/>
+      <c r="J11" s="60"/>
+      <c r="K11" s="70" t="s">
         <v>1</v>
       </c>
-      <c r="L11" s="43"/>
-      <c r="M11" s="43"/>
-      <c r="N11" s="43"/>
-      <c r="O11" s="43"/>
-      <c r="P11" s="43"/>
-      <c r="Q11" s="43"/>
-      <c r="R11" s="56"/>
-      <c r="S11" s="58" t="s">
+      <c r="L11" s="51"/>
+      <c r="M11" s="51"/>
+      <c r="N11" s="51"/>
+      <c r="O11" s="51"/>
+      <c r="P11" s="51"/>
+      <c r="Q11" s="51"/>
+      <c r="R11" s="68"/>
+      <c r="S11" s="71" t="s">
         <v>2</v>
       </c>
-      <c r="T11" s="43"/>
-      <c r="U11" s="43"/>
-      <c r="V11" s="43"/>
-      <c r="W11" s="43"/>
-      <c r="X11" s="43"/>
-      <c r="Y11" s="43"/>
-      <c r="Z11" s="43"/>
-      <c r="AA11" s="43"/>
-      <c r="AB11" s="43"/>
-      <c r="AC11" s="44"/>
-      <c r="AD11" s="46" t="s">
+      <c r="T11" s="51"/>
+      <c r="U11" s="51"/>
+      <c r="V11" s="51"/>
+      <c r="W11" s="51"/>
+      <c r="X11" s="51"/>
+      <c r="Y11" s="51"/>
+      <c r="Z11" s="51"/>
+      <c r="AA11" s="51"/>
+      <c r="AB11" s="51"/>
+      <c r="AC11" s="28"/>
+      <c r="AD11" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="AE11" s="35"/>
-      <c r="AF11" s="36"/>
-      <c r="AG11" s="45" t="s">
+      <c r="AE11" s="59"/>
+      <c r="AF11" s="60"/>
+      <c r="AG11" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="AH11" s="45" t="s">
+      <c r="AH11" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="AI11" s="45" t="s">
+      <c r="AI11" s="48" t="s">
         <v>46</v>
       </c>
       <c r="AJ11" s="6"/>
@@ -1700,50 +1710,50 @@
       <c r="AO11" s="6"/>
       <c r="AP11" s="6"/>
     </row>
-    <row r="12" spans="1:42" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:42" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
-      <c r="B12" s="32"/>
-      <c r="C12" s="60"/>
-      <c r="D12" s="73"/>
-      <c r="E12" s="78"/>
-      <c r="F12" s="79"/>
-      <c r="G12" s="80"/>
-      <c r="H12" s="37"/>
-      <c r="I12" s="38"/>
-      <c r="J12" s="39"/>
-      <c r="K12" s="55" t="s">
+      <c r="B12" s="49"/>
+      <c r="C12" s="76"/>
+      <c r="D12" s="32"/>
+      <c r="E12" s="38"/>
+      <c r="F12" s="39"/>
+      <c r="G12" s="40"/>
+      <c r="H12" s="61"/>
+      <c r="I12" s="62"/>
+      <c r="J12" s="63"/>
+      <c r="K12" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="L12" s="43"/>
-      <c r="M12" s="43"/>
-      <c r="N12" s="43"/>
-      <c r="O12" s="43"/>
-      <c r="P12" s="43"/>
-      <c r="Q12" s="43"/>
-      <c r="R12" s="56"/>
-      <c r="S12" s="42" t="s">
+      <c r="L12" s="51"/>
+      <c r="M12" s="51"/>
+      <c r="N12" s="51"/>
+      <c r="O12" s="51"/>
+      <c r="P12" s="51"/>
+      <c r="Q12" s="51"/>
+      <c r="R12" s="68"/>
+      <c r="S12" s="69" t="s">
         <v>10</v>
       </c>
-      <c r="T12" s="43"/>
-      <c r="U12" s="44"/>
-      <c r="V12" s="42" t="s">
+      <c r="T12" s="51"/>
+      <c r="U12" s="28"/>
+      <c r="V12" s="69" t="s">
         <v>11</v>
       </c>
-      <c r="W12" s="43"/>
-      <c r="X12" s="43"/>
-      <c r="Y12" s="43"/>
-      <c r="Z12" s="43"/>
-      <c r="AA12" s="43"/>
-      <c r="AB12" s="44"/>
-      <c r="AC12" s="31" t="s">
+      <c r="W12" s="51"/>
+      <c r="X12" s="51"/>
+      <c r="Y12" s="51"/>
+      <c r="Z12" s="51"/>
+      <c r="AA12" s="51"/>
+      <c r="AB12" s="28"/>
+      <c r="AC12" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="AD12" s="37"/>
-      <c r="AE12" s="38"/>
-      <c r="AF12" s="39"/>
-      <c r="AG12" s="32"/>
-      <c r="AH12" s="32"/>
-      <c r="AI12" s="32"/>
+      <c r="AD12" s="61"/>
+      <c r="AE12" s="62"/>
+      <c r="AF12" s="63"/>
+      <c r="AG12" s="49"/>
+      <c r="AH12" s="49"/>
+      <c r="AI12" s="49"/>
       <c r="AJ12" s="7"/>
       <c r="AK12" s="7"/>
       <c r="AL12" s="7"/>
@@ -1752,78 +1762,78 @@
       <c r="AO12" s="7"/>
       <c r="AP12" s="7"/>
     </row>
-    <row r="13" spans="1:42" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:42" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
-      <c r="B13" s="32"/>
-      <c r="C13" s="60"/>
-      <c r="D13" s="74"/>
-      <c r="E13" s="83" t="s">
+      <c r="B13" s="49"/>
+      <c r="C13" s="76"/>
+      <c r="D13" s="33"/>
+      <c r="E13" s="45" t="s">
         <v>22</v>
       </c>
-      <c r="F13" s="83"/>
-      <c r="G13" s="48" t="s">
+      <c r="F13" s="45"/>
+      <c r="G13" s="65" t="s">
         <v>49</v>
       </c>
-      <c r="H13" s="51" t="s">
+      <c r="H13" s="66" t="s">
         <v>6</v>
       </c>
-      <c r="I13" s="31" t="s">
+      <c r="I13" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="J13" s="31" t="s">
+      <c r="J13" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="K13" s="55" t="s">
+      <c r="K13" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="L13" s="43"/>
-      <c r="M13" s="43"/>
-      <c r="N13" s="43"/>
-      <c r="O13" s="43"/>
-      <c r="P13" s="43"/>
-      <c r="Q13" s="43"/>
-      <c r="R13" s="44"/>
-      <c r="S13" s="45" t="s">
+      <c r="L13" s="51"/>
+      <c r="M13" s="51"/>
+      <c r="N13" s="51"/>
+      <c r="O13" s="51"/>
+      <c r="P13" s="51"/>
+      <c r="Q13" s="51"/>
+      <c r="R13" s="28"/>
+      <c r="S13" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="T13" s="45" t="s">
+      <c r="T13" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="U13" s="31" t="s">
+      <c r="U13" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="V13" s="47" t="s">
+      <c r="V13" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="W13" s="45" t="s">
+      <c r="W13" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="X13" s="31" t="s">
+      <c r="X13" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="Y13" s="31" t="s">
+      <c r="Y13" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="Z13" s="31" t="s">
+      <c r="Z13" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="AA13" s="31" t="s">
+      <c r="AA13" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="AB13" s="31" t="s">
+      <c r="AB13" s="46" t="s">
         <v>21</v>
       </c>
-      <c r="AC13" s="32"/>
-      <c r="AD13" s="63" t="s">
+      <c r="AC13" s="49"/>
+      <c r="AD13" s="52" t="s">
         <v>36</v>
       </c>
-      <c r="AE13" s="71" t="s">
+      <c r="AE13" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="AF13" s="44"/>
-      <c r="AG13" s="32"/>
-      <c r="AH13" s="32"/>
-      <c r="AI13" s="32"/>
+      <c r="AF13" s="28"/>
+      <c r="AG13" s="49"/>
+      <c r="AH13" s="49"/>
+      <c r="AI13" s="49"/>
       <c r="AJ13" s="6"/>
       <c r="AK13" s="6"/>
       <c r="AL13" s="6"/>
@@ -1832,60 +1842,60 @@
       <c r="AO13" s="6"/>
       <c r="AP13" s="7"/>
     </row>
-    <row r="14" spans="1:42" ht="68.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:42" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
-      <c r="B14" s="32"/>
-      <c r="C14" s="60"/>
-      <c r="D14" s="74"/>
-      <c r="E14" s="49" t="s">
+      <c r="B14" s="49"/>
+      <c r="C14" s="76"/>
+      <c r="D14" s="33"/>
+      <c r="E14" s="43" t="s">
         <v>51</v>
       </c>
-      <c r="F14" s="81" t="s">
+      <c r="F14" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="G14" s="49"/>
-      <c r="H14" s="52"/>
-      <c r="I14" s="32"/>
-      <c r="J14" s="32"/>
-      <c r="K14" s="31" t="s">
+      <c r="G14" s="43"/>
+      <c r="H14" s="67"/>
+      <c r="I14" s="49"/>
+      <c r="J14" s="49"/>
+      <c r="K14" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="L14" s="54" t="s">
+      <c r="L14" s="55" t="s">
         <v>25</v>
       </c>
-      <c r="M14" s="43"/>
-      <c r="N14" s="44"/>
-      <c r="O14" s="54" t="s">
+      <c r="M14" s="51"/>
+      <c r="N14" s="28"/>
+      <c r="O14" s="55" t="s">
         <v>37</v>
       </c>
-      <c r="P14" s="44"/>
-      <c r="Q14" s="27" t="s">
+      <c r="P14" s="28"/>
+      <c r="Q14" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="R14" s="27" t="s">
+      <c r="R14" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="S14" s="32"/>
-      <c r="T14" s="32"/>
-      <c r="U14" s="32"/>
-      <c r="V14" s="32"/>
-      <c r="W14" s="32"/>
-      <c r="X14" s="32"/>
-      <c r="Y14" s="32"/>
-      <c r="Z14" s="32"/>
-      <c r="AA14" s="32"/>
-      <c r="AB14" s="32"/>
-      <c r="AC14" s="32"/>
-      <c r="AD14" s="64"/>
-      <c r="AE14" s="31" t="s">
+      <c r="S14" s="49"/>
+      <c r="T14" s="49"/>
+      <c r="U14" s="49"/>
+      <c r="V14" s="49"/>
+      <c r="W14" s="49"/>
+      <c r="X14" s="49"/>
+      <c r="Y14" s="49"/>
+      <c r="Z14" s="49"/>
+      <c r="AA14" s="49"/>
+      <c r="AB14" s="49"/>
+      <c r="AC14" s="49"/>
+      <c r="AD14" s="53"/>
+      <c r="AE14" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="AF14" s="31" t="s">
+      <c r="AF14" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="AG14" s="32"/>
-      <c r="AH14" s="32"/>
-      <c r="AI14" s="32"/>
+      <c r="AG14" s="49"/>
+      <c r="AH14" s="49"/>
+      <c r="AI14" s="49"/>
       <c r="AJ14" s="6"/>
       <c r="AK14" s="6"/>
       <c r="AL14" s="6"/>
@@ -1894,18 +1904,18 @@
       <c r="AO14" s="6"/>
       <c r="AP14" s="7"/>
     </row>
-    <row r="15" spans="1:42" ht="52.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:42" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
-      <c r="B15" s="33"/>
-      <c r="C15" s="61"/>
-      <c r="D15" s="75"/>
-      <c r="E15" s="50"/>
-      <c r="F15" s="82"/>
-      <c r="G15" s="50"/>
-      <c r="H15" s="39"/>
-      <c r="I15" s="33"/>
-      <c r="J15" s="33"/>
-      <c r="K15" s="33"/>
+      <c r="B15" s="24"/>
+      <c r="C15" s="77"/>
+      <c r="D15" s="34"/>
+      <c r="E15" s="44"/>
+      <c r="F15" s="42"/>
+      <c r="G15" s="44"/>
+      <c r="H15" s="63"/>
+      <c r="I15" s="24"/>
+      <c r="J15" s="24"/>
+      <c r="K15" s="24"/>
       <c r="L15" s="8">
         <v>0</v>
       </c>
@@ -1924,26 +1934,26 @@
       <c r="Q15" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="R15" s="28" t="s">
+      <c r="R15" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="S15" s="33"/>
-      <c r="T15" s="33"/>
-      <c r="U15" s="33"/>
-      <c r="V15" s="33"/>
-      <c r="W15" s="33"/>
-      <c r="X15" s="33"/>
-      <c r="Y15" s="33"/>
-      <c r="Z15" s="33"/>
-      <c r="AA15" s="33"/>
-      <c r="AB15" s="33"/>
-      <c r="AC15" s="33"/>
-      <c r="AD15" s="65"/>
-      <c r="AE15" s="33"/>
-      <c r="AF15" s="33"/>
-      <c r="AG15" s="33"/>
-      <c r="AH15" s="33"/>
-      <c r="AI15" s="33"/>
+      <c r="S15" s="24"/>
+      <c r="T15" s="24"/>
+      <c r="U15" s="24"/>
+      <c r="V15" s="24"/>
+      <c r="W15" s="24"/>
+      <c r="X15" s="24"/>
+      <c r="Y15" s="24"/>
+      <c r="Z15" s="24"/>
+      <c r="AA15" s="24"/>
+      <c r="AB15" s="24"/>
+      <c r="AC15" s="24"/>
+      <c r="AD15" s="54"/>
+      <c r="AE15" s="24"/>
+      <c r="AF15" s="24"/>
+      <c r="AG15" s="24"/>
+      <c r="AH15" s="24"/>
+      <c r="AI15" s="24"/>
       <c r="AJ15" s="6"/>
       <c r="AK15" s="6"/>
       <c r="AL15" s="6"/>
@@ -1952,7 +1962,7 @@
       <c r="AO15" s="6"/>
       <c r="AP15" s="7"/>
     </row>
-    <row r="16" spans="1:42" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:42" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="9">
         <v>3</v>
@@ -2056,7 +2066,7 @@
       <c r="AI16" s="10">
         <v>36</v>
       </c>
-      <c r="AJ16" s="12"/>
+      <c r="AJ16" s="11"/>
       <c r="AK16" s="7"/>
       <c r="AL16" s="7"/>
       <c r="AM16" s="7"/>
@@ -2064,46 +2074,46 @@
       <c r="AO16" s="7"/>
       <c r="AP16" s="7"/>
     </row>
-    <row r="17" spans="1:42" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:42" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
-      <c r="B17" s="69" t="s">
+      <c r="B17" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="C17" s="13" t="s">
+      <c r="C17" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="11"/>
-      <c r="I17" s="11"/>
-      <c r="J17" s="11"/>
-      <c r="K17" s="9"/>
-      <c r="L17" s="9"/>
-      <c r="M17" s="9"/>
-      <c r="N17" s="9"/>
-      <c r="O17" s="10"/>
-      <c r="P17" s="10"/>
-      <c r="Q17" s="10"/>
-      <c r="R17" s="10"/>
-      <c r="S17" s="10"/>
-      <c r="T17" s="10"/>
-      <c r="U17" s="10"/>
-      <c r="V17" s="10"/>
-      <c r="W17" s="10"/>
-      <c r="X17" s="10"/>
-      <c r="Y17" s="10"/>
-      <c r="Z17" s="10"/>
-      <c r="AA17" s="10"/>
-      <c r="AB17" s="10"/>
-      <c r="AC17" s="10"/>
-      <c r="AD17" s="10"/>
-      <c r="AE17" s="10"/>
-      <c r="AF17" s="10"/>
-      <c r="AG17" s="10"/>
-      <c r="AH17" s="10"/>
-      <c r="AI17" s="10"/>
+      <c r="D17" s="80"/>
+      <c r="E17" s="80"/>
+      <c r="F17" s="81"/>
+      <c r="G17" s="82"/>
+      <c r="H17" s="83"/>
+      <c r="I17" s="83"/>
+      <c r="J17" s="83"/>
+      <c r="K17" s="81"/>
+      <c r="L17" s="81"/>
+      <c r="M17" s="81"/>
+      <c r="N17" s="81"/>
+      <c r="O17" s="82"/>
+      <c r="P17" s="82"/>
+      <c r="Q17" s="82"/>
+      <c r="R17" s="82"/>
+      <c r="S17" s="82"/>
+      <c r="T17" s="82"/>
+      <c r="U17" s="82"/>
+      <c r="V17" s="82"/>
+      <c r="W17" s="82"/>
+      <c r="X17" s="82"/>
+      <c r="Y17" s="82"/>
+      <c r="Z17" s="82"/>
+      <c r="AA17" s="82"/>
+      <c r="AB17" s="82"/>
+      <c r="AC17" s="82"/>
+      <c r="AD17" s="82"/>
+      <c r="AE17" s="82"/>
+      <c r="AF17" s="82"/>
+      <c r="AG17" s="82"/>
+      <c r="AH17" s="82"/>
+      <c r="AI17" s="82"/>
       <c r="AJ17" s="7"/>
       <c r="AK17" s="7"/>
       <c r="AL17" s="7"/>
@@ -2112,44 +2122,44 @@
       <c r="AO17" s="7"/>
       <c r="AP17" s="7"/>
     </row>
-    <row r="18" spans="1:42" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:42" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
-      <c r="B18" s="70"/>
-      <c r="C18" s="13" t="s">
+      <c r="B18" s="26"/>
+      <c r="C18" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="11"/>
-      <c r="I18" s="11"/>
-      <c r="J18" s="11"/>
-      <c r="K18" s="9"/>
-      <c r="L18" s="9"/>
-      <c r="M18" s="9"/>
-      <c r="N18" s="9"/>
-      <c r="O18" s="10"/>
-      <c r="P18" s="10"/>
-      <c r="Q18" s="10"/>
-      <c r="R18" s="10"/>
-      <c r="S18" s="10"/>
-      <c r="T18" s="10"/>
-      <c r="U18" s="10"/>
-      <c r="V18" s="10"/>
-      <c r="W18" s="10"/>
-      <c r="X18" s="10"/>
-      <c r="Y18" s="10"/>
-      <c r="Z18" s="10"/>
-      <c r="AA18" s="10"/>
-      <c r="AB18" s="10"/>
-      <c r="AC18" s="10"/>
-      <c r="AD18" s="10"/>
-      <c r="AE18" s="10"/>
-      <c r="AF18" s="10"/>
-      <c r="AG18" s="10"/>
-      <c r="AH18" s="10"/>
-      <c r="AI18" s="10"/>
+      <c r="D18" s="80"/>
+      <c r="E18" s="80"/>
+      <c r="F18" s="81"/>
+      <c r="G18" s="82"/>
+      <c r="H18" s="83"/>
+      <c r="I18" s="83"/>
+      <c r="J18" s="83"/>
+      <c r="K18" s="81"/>
+      <c r="L18" s="81"/>
+      <c r="M18" s="81"/>
+      <c r="N18" s="81"/>
+      <c r="O18" s="82"/>
+      <c r="P18" s="82"/>
+      <c r="Q18" s="82"/>
+      <c r="R18" s="82"/>
+      <c r="S18" s="82"/>
+      <c r="T18" s="82"/>
+      <c r="U18" s="82"/>
+      <c r="V18" s="82"/>
+      <c r="W18" s="82"/>
+      <c r="X18" s="82"/>
+      <c r="Y18" s="82"/>
+      <c r="Z18" s="82"/>
+      <c r="AA18" s="82"/>
+      <c r="AB18" s="82"/>
+      <c r="AC18" s="82"/>
+      <c r="AD18" s="82"/>
+      <c r="AE18" s="82"/>
+      <c r="AF18" s="82"/>
+      <c r="AG18" s="82"/>
+      <c r="AH18" s="82"/>
+      <c r="AI18" s="82"/>
       <c r="AJ18" s="7"/>
       <c r="AK18" s="7"/>
       <c r="AL18" s="7"/>
@@ -2158,46 +2168,46 @@
       <c r="AO18" s="7"/>
       <c r="AP18" s="7"/>
     </row>
-    <row r="19" spans="1:42" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:42" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
-      <c r="B19" s="68" t="s">
+      <c r="B19" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="C19" s="13" t="s">
+      <c r="C19" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="9"/>
-      <c r="H19" s="14"/>
-      <c r="I19" s="14"/>
-      <c r="J19" s="14"/>
-      <c r="K19" s="9"/>
-      <c r="L19" s="10"/>
-      <c r="M19" s="9"/>
-      <c r="N19" s="10"/>
-      <c r="O19" s="9"/>
-      <c r="P19" s="10"/>
-      <c r="Q19" s="10"/>
-      <c r="R19" s="10"/>
-      <c r="S19" s="9"/>
-      <c r="T19" s="10"/>
-      <c r="U19" s="9"/>
-      <c r="V19" s="10"/>
-      <c r="W19" s="10"/>
-      <c r="X19" s="10"/>
-      <c r="Y19" s="10"/>
-      <c r="Z19" s="10"/>
-      <c r="AA19" s="10"/>
-      <c r="AB19" s="10"/>
-      <c r="AC19" s="10"/>
-      <c r="AD19" s="10"/>
-      <c r="AE19" s="10"/>
-      <c r="AF19" s="9"/>
-      <c r="AG19" s="10"/>
-      <c r="AH19" s="9"/>
-      <c r="AI19" s="10"/>
+      <c r="D19" s="80"/>
+      <c r="E19" s="80"/>
+      <c r="F19" s="80"/>
+      <c r="G19" s="81"/>
+      <c r="H19" s="84"/>
+      <c r="I19" s="84"/>
+      <c r="J19" s="84"/>
+      <c r="K19" s="81"/>
+      <c r="L19" s="82"/>
+      <c r="M19" s="81"/>
+      <c r="N19" s="82"/>
+      <c r="O19" s="81"/>
+      <c r="P19" s="82"/>
+      <c r="Q19" s="82"/>
+      <c r="R19" s="82"/>
+      <c r="S19" s="81"/>
+      <c r="T19" s="82"/>
+      <c r="U19" s="81"/>
+      <c r="V19" s="82"/>
+      <c r="W19" s="82"/>
+      <c r="X19" s="82"/>
+      <c r="Y19" s="82"/>
+      <c r="Z19" s="82"/>
+      <c r="AA19" s="82"/>
+      <c r="AB19" s="82"/>
+      <c r="AC19" s="82"/>
+      <c r="AD19" s="82"/>
+      <c r="AE19" s="82"/>
+      <c r="AF19" s="81"/>
+      <c r="AG19" s="82"/>
+      <c r="AH19" s="81"/>
+      <c r="AI19" s="82"/>
       <c r="AJ19" s="7"/>
       <c r="AK19" s="7"/>
       <c r="AL19" s="7"/>
@@ -2206,44 +2216,44 @@
       <c r="AO19" s="7"/>
       <c r="AP19" s="7"/>
     </row>
-    <row r="20" spans="1:42" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:42" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
-      <c r="B20" s="33"/>
-      <c r="C20" s="13" t="s">
+      <c r="B20" s="24"/>
+      <c r="C20" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="15"/>
-      <c r="H20" s="16"/>
-      <c r="I20" s="16"/>
-      <c r="J20" s="16"/>
-      <c r="K20" s="15"/>
-      <c r="L20" s="15"/>
-      <c r="M20" s="15"/>
-      <c r="N20" s="15"/>
-      <c r="O20" s="15"/>
-      <c r="P20" s="15"/>
-      <c r="Q20" s="15"/>
-      <c r="R20" s="15"/>
-      <c r="S20" s="17"/>
-      <c r="T20" s="17"/>
-      <c r="U20" s="17"/>
-      <c r="V20" s="17"/>
-      <c r="W20" s="17"/>
-      <c r="X20" s="17"/>
-      <c r="Y20" s="17"/>
-      <c r="Z20" s="17"/>
-      <c r="AA20" s="17"/>
-      <c r="AB20" s="17"/>
-      <c r="AC20" s="17"/>
-      <c r="AD20" s="17"/>
-      <c r="AE20" s="17"/>
-      <c r="AF20" s="17"/>
-      <c r="AG20" s="17"/>
-      <c r="AH20" s="17"/>
-      <c r="AI20" s="18"/>
+      <c r="D20" s="80"/>
+      <c r="E20" s="80"/>
+      <c r="F20" s="80"/>
+      <c r="G20" s="78"/>
+      <c r="H20" s="79"/>
+      <c r="I20" s="79"/>
+      <c r="J20" s="79"/>
+      <c r="K20" s="78"/>
+      <c r="L20" s="78"/>
+      <c r="M20" s="78"/>
+      <c r="N20" s="78"/>
+      <c r="O20" s="78"/>
+      <c r="P20" s="78"/>
+      <c r="Q20" s="78"/>
+      <c r="R20" s="78"/>
+      <c r="S20" s="80"/>
+      <c r="T20" s="80"/>
+      <c r="U20" s="80"/>
+      <c r="V20" s="80"/>
+      <c r="W20" s="80"/>
+      <c r="X20" s="80"/>
+      <c r="Y20" s="80"/>
+      <c r="Z20" s="80"/>
+      <c r="AA20" s="80"/>
+      <c r="AB20" s="80"/>
+      <c r="AC20" s="80"/>
+      <c r="AD20" s="80"/>
+      <c r="AE20" s="80"/>
+      <c r="AF20" s="80"/>
+      <c r="AG20" s="80"/>
+      <c r="AH20" s="80"/>
+      <c r="AI20" s="85"/>
       <c r="AJ20" s="1"/>
       <c r="AK20" s="1"/>
       <c r="AL20" s="1"/>
@@ -2252,46 +2262,46 @@
       <c r="AO20" s="1"/>
       <c r="AP20" s="1"/>
     </row>
-    <row r="21" spans="1:42" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:42" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
-      <c r="B21" s="68" t="s">
+      <c r="B21" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="C21" s="13" t="s">
+      <c r="C21" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="15"/>
-      <c r="H21" s="16"/>
-      <c r="I21" s="16"/>
-      <c r="J21" s="16"/>
-      <c r="K21" s="15"/>
-      <c r="L21" s="15"/>
-      <c r="M21" s="15"/>
-      <c r="N21" s="15"/>
-      <c r="O21" s="15"/>
-      <c r="P21" s="15"/>
-      <c r="Q21" s="15"/>
-      <c r="R21" s="15"/>
-      <c r="S21" s="17"/>
-      <c r="T21" s="17"/>
-      <c r="U21" s="17"/>
-      <c r="V21" s="17"/>
-      <c r="W21" s="17"/>
-      <c r="X21" s="17"/>
-      <c r="Y21" s="17"/>
-      <c r="Z21" s="17"/>
-      <c r="AA21" s="17"/>
-      <c r="AB21" s="17"/>
-      <c r="AC21" s="17"/>
-      <c r="AD21" s="17"/>
-      <c r="AE21" s="17"/>
-      <c r="AF21" s="17"/>
-      <c r="AG21" s="17"/>
-      <c r="AH21" s="17"/>
-      <c r="AI21" s="18"/>
+      <c r="D21" s="80"/>
+      <c r="E21" s="80"/>
+      <c r="F21" s="80"/>
+      <c r="G21" s="78"/>
+      <c r="H21" s="79"/>
+      <c r="I21" s="79"/>
+      <c r="J21" s="79"/>
+      <c r="K21" s="78"/>
+      <c r="L21" s="78"/>
+      <c r="M21" s="78"/>
+      <c r="N21" s="78"/>
+      <c r="O21" s="78"/>
+      <c r="P21" s="78"/>
+      <c r="Q21" s="78"/>
+      <c r="R21" s="78"/>
+      <c r="S21" s="80"/>
+      <c r="T21" s="80"/>
+      <c r="U21" s="80"/>
+      <c r="V21" s="80"/>
+      <c r="W21" s="80"/>
+      <c r="X21" s="80"/>
+      <c r="Y21" s="80"/>
+      <c r="Z21" s="80"/>
+      <c r="AA21" s="80"/>
+      <c r="AB21" s="80"/>
+      <c r="AC21" s="80"/>
+      <c r="AD21" s="80"/>
+      <c r="AE21" s="80"/>
+      <c r="AF21" s="80"/>
+      <c r="AG21" s="80"/>
+      <c r="AH21" s="80"/>
+      <c r="AI21" s="85"/>
       <c r="AJ21" s="1"/>
       <c r="AK21" s="1"/>
       <c r="AL21" s="1"/>
@@ -2300,44 +2310,44 @@
       <c r="AO21" s="1"/>
       <c r="AP21" s="1"/>
     </row>
-    <row r="22" spans="1:42" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:42" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
-      <c r="B22" s="33"/>
-      <c r="C22" s="13" t="s">
+      <c r="B22" s="24"/>
+      <c r="C22" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="15"/>
-      <c r="H22" s="16"/>
-      <c r="I22" s="16"/>
-      <c r="J22" s="16"/>
-      <c r="K22" s="15"/>
-      <c r="L22" s="15"/>
-      <c r="M22" s="15"/>
-      <c r="N22" s="15"/>
-      <c r="O22" s="15"/>
-      <c r="P22" s="15"/>
-      <c r="Q22" s="15"/>
-      <c r="R22" s="15"/>
-      <c r="S22" s="17"/>
-      <c r="T22" s="17"/>
-      <c r="U22" s="17"/>
-      <c r="V22" s="17"/>
-      <c r="W22" s="17"/>
-      <c r="X22" s="17"/>
-      <c r="Y22" s="17"/>
-      <c r="Z22" s="17"/>
-      <c r="AA22" s="17"/>
-      <c r="AB22" s="17"/>
-      <c r="AC22" s="17"/>
-      <c r="AD22" s="17"/>
-      <c r="AE22" s="17"/>
-      <c r="AF22" s="17"/>
-      <c r="AG22" s="17"/>
-      <c r="AH22" s="17"/>
-      <c r="AI22" s="18"/>
+      <c r="D22" s="80"/>
+      <c r="E22" s="80"/>
+      <c r="F22" s="80"/>
+      <c r="G22" s="78"/>
+      <c r="H22" s="79"/>
+      <c r="I22" s="79"/>
+      <c r="J22" s="79"/>
+      <c r="K22" s="78"/>
+      <c r="L22" s="78"/>
+      <c r="M22" s="78"/>
+      <c r="N22" s="78"/>
+      <c r="O22" s="78"/>
+      <c r="P22" s="78"/>
+      <c r="Q22" s="78"/>
+      <c r="R22" s="78"/>
+      <c r="S22" s="80"/>
+      <c r="T22" s="80"/>
+      <c r="U22" s="80"/>
+      <c r="V22" s="80"/>
+      <c r="W22" s="80"/>
+      <c r="X22" s="80"/>
+      <c r="Y22" s="80"/>
+      <c r="Z22" s="80"/>
+      <c r="AA22" s="80"/>
+      <c r="AB22" s="80"/>
+      <c r="AC22" s="80"/>
+      <c r="AD22" s="80"/>
+      <c r="AE22" s="80"/>
+      <c r="AF22" s="80"/>
+      <c r="AG22" s="80"/>
+      <c r="AH22" s="80"/>
+      <c r="AI22" s="85"/>
       <c r="AJ22" s="1"/>
       <c r="AK22" s="1"/>
       <c r="AL22" s="1"/>
@@ -2346,46 +2356,46 @@
       <c r="AO22" s="1"/>
       <c r="AP22" s="1"/>
     </row>
-    <row r="23" spans="1:42" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:42" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
-      <c r="B23" s="68" t="s">
+      <c r="B23" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="C23" s="13" t="s">
+      <c r="C23" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="15"/>
-      <c r="H23" s="16"/>
-      <c r="I23" s="16"/>
-      <c r="J23" s="16"/>
-      <c r="K23" s="15"/>
-      <c r="L23" s="15"/>
-      <c r="M23" s="15"/>
-      <c r="N23" s="15"/>
-      <c r="O23" s="15"/>
-      <c r="P23" s="15"/>
-      <c r="Q23" s="15"/>
-      <c r="R23" s="15"/>
-      <c r="S23" s="17"/>
-      <c r="T23" s="17"/>
-      <c r="U23" s="17"/>
-      <c r="V23" s="17"/>
-      <c r="W23" s="17"/>
-      <c r="X23" s="17"/>
-      <c r="Y23" s="17"/>
-      <c r="Z23" s="17"/>
-      <c r="AA23" s="17"/>
-      <c r="AB23" s="17"/>
-      <c r="AC23" s="17"/>
-      <c r="AD23" s="17"/>
-      <c r="AE23" s="17"/>
-      <c r="AF23" s="17"/>
-      <c r="AG23" s="17"/>
-      <c r="AH23" s="17"/>
-      <c r="AI23" s="18"/>
+      <c r="D23" s="80"/>
+      <c r="E23" s="80"/>
+      <c r="F23" s="80"/>
+      <c r="G23" s="78"/>
+      <c r="H23" s="79"/>
+      <c r="I23" s="79"/>
+      <c r="J23" s="79"/>
+      <c r="K23" s="78"/>
+      <c r="L23" s="78"/>
+      <c r="M23" s="78"/>
+      <c r="N23" s="78"/>
+      <c r="O23" s="78"/>
+      <c r="P23" s="78"/>
+      <c r="Q23" s="78"/>
+      <c r="R23" s="78"/>
+      <c r="S23" s="80"/>
+      <c r="T23" s="80"/>
+      <c r="U23" s="80"/>
+      <c r="V23" s="80"/>
+      <c r="W23" s="80"/>
+      <c r="X23" s="80"/>
+      <c r="Y23" s="80"/>
+      <c r="Z23" s="80"/>
+      <c r="AA23" s="80"/>
+      <c r="AB23" s="80"/>
+      <c r="AC23" s="80"/>
+      <c r="AD23" s="80"/>
+      <c r="AE23" s="80"/>
+      <c r="AF23" s="80"/>
+      <c r="AG23" s="80"/>
+      <c r="AH23" s="80"/>
+      <c r="AI23" s="85"/>
       <c r="AJ23" s="1"/>
       <c r="AK23" s="1"/>
       <c r="AL23" s="1"/>
@@ -2394,44 +2404,44 @@
       <c r="AO23" s="1"/>
       <c r="AP23" s="1"/>
     </row>
-    <row r="24" spans="1:42" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:42" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
-      <c r="B24" s="33"/>
-      <c r="C24" s="13" t="s">
+      <c r="B24" s="24"/>
+      <c r="C24" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="15"/>
-      <c r="H24" s="16"/>
-      <c r="I24" s="16"/>
-      <c r="J24" s="16"/>
-      <c r="K24" s="15"/>
-      <c r="L24" s="15"/>
-      <c r="M24" s="15"/>
-      <c r="N24" s="15"/>
-      <c r="O24" s="15"/>
-      <c r="P24" s="15"/>
-      <c r="Q24" s="15"/>
-      <c r="R24" s="15"/>
-      <c r="S24" s="17"/>
-      <c r="T24" s="17"/>
-      <c r="U24" s="17"/>
-      <c r="V24" s="17"/>
-      <c r="W24" s="17"/>
-      <c r="X24" s="17"/>
-      <c r="Y24" s="17"/>
-      <c r="Z24" s="17"/>
-      <c r="AA24" s="17"/>
-      <c r="AB24" s="17"/>
-      <c r="AC24" s="17"/>
-      <c r="AD24" s="17"/>
-      <c r="AE24" s="17"/>
-      <c r="AF24" s="17"/>
-      <c r="AG24" s="17"/>
-      <c r="AH24" s="17"/>
-      <c r="AI24" s="17"/>
+      <c r="D24" s="80"/>
+      <c r="E24" s="80"/>
+      <c r="F24" s="80"/>
+      <c r="G24" s="78"/>
+      <c r="H24" s="79"/>
+      <c r="I24" s="79"/>
+      <c r="J24" s="79"/>
+      <c r="K24" s="78"/>
+      <c r="L24" s="78"/>
+      <c r="M24" s="78"/>
+      <c r="N24" s="78"/>
+      <c r="O24" s="78"/>
+      <c r="P24" s="78"/>
+      <c r="Q24" s="78"/>
+      <c r="R24" s="78"/>
+      <c r="S24" s="80"/>
+      <c r="T24" s="80"/>
+      <c r="U24" s="80"/>
+      <c r="V24" s="80"/>
+      <c r="W24" s="80"/>
+      <c r="X24" s="80"/>
+      <c r="Y24" s="80"/>
+      <c r="Z24" s="80"/>
+      <c r="AA24" s="80"/>
+      <c r="AB24" s="80"/>
+      <c r="AC24" s="80"/>
+      <c r="AD24" s="80"/>
+      <c r="AE24" s="80"/>
+      <c r="AF24" s="80"/>
+      <c r="AG24" s="80"/>
+      <c r="AH24" s="80"/>
+      <c r="AI24" s="80"/>
       <c r="AJ24" s="1"/>
       <c r="AK24" s="1"/>
       <c r="AL24" s="1"/>
@@ -2440,46 +2450,46 @@
       <c r="AO24" s="1"/>
       <c r="AP24" s="1"/>
     </row>
-    <row r="25" spans="1:42" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:42" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
-      <c r="B25" s="68" t="s">
+      <c r="B25" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="C25" s="13" t="s">
+      <c r="C25" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="15"/>
-      <c r="H25" s="16"/>
-      <c r="I25" s="16"/>
-      <c r="J25" s="16"/>
-      <c r="K25" s="15"/>
-      <c r="L25" s="15"/>
-      <c r="M25" s="15"/>
-      <c r="N25" s="15"/>
-      <c r="O25" s="15"/>
-      <c r="P25" s="15"/>
-      <c r="Q25" s="15"/>
-      <c r="R25" s="15"/>
-      <c r="S25" s="17"/>
-      <c r="T25" s="17"/>
-      <c r="U25" s="17"/>
-      <c r="V25" s="17"/>
-      <c r="W25" s="17"/>
-      <c r="X25" s="17"/>
-      <c r="Y25" s="17"/>
-      <c r="Z25" s="17"/>
-      <c r="AA25" s="17"/>
-      <c r="AB25" s="17"/>
-      <c r="AC25" s="17"/>
-      <c r="AD25" s="17"/>
-      <c r="AE25" s="17"/>
-      <c r="AF25" s="17"/>
-      <c r="AG25" s="17"/>
-      <c r="AH25" s="17"/>
-      <c r="AI25" s="17"/>
+      <c r="D25" s="80"/>
+      <c r="E25" s="80"/>
+      <c r="F25" s="80"/>
+      <c r="G25" s="78"/>
+      <c r="H25" s="79"/>
+      <c r="I25" s="79"/>
+      <c r="J25" s="79"/>
+      <c r="K25" s="78"/>
+      <c r="L25" s="78"/>
+      <c r="M25" s="78"/>
+      <c r="N25" s="78"/>
+      <c r="O25" s="78"/>
+      <c r="P25" s="78"/>
+      <c r="Q25" s="78"/>
+      <c r="R25" s="78"/>
+      <c r="S25" s="80"/>
+      <c r="T25" s="80"/>
+      <c r="U25" s="80"/>
+      <c r="V25" s="80"/>
+      <c r="W25" s="80"/>
+      <c r="X25" s="80"/>
+      <c r="Y25" s="80"/>
+      <c r="Z25" s="80"/>
+      <c r="AA25" s="80"/>
+      <c r="AB25" s="80"/>
+      <c r="AC25" s="80"/>
+      <c r="AD25" s="80"/>
+      <c r="AE25" s="80"/>
+      <c r="AF25" s="80"/>
+      <c r="AG25" s="80"/>
+      <c r="AH25" s="80"/>
+      <c r="AI25" s="80"/>
       <c r="AJ25" s="1"/>
       <c r="AK25" s="1"/>
       <c r="AL25" s="1"/>
@@ -2488,44 +2498,44 @@
       <c r="AO25" s="1"/>
       <c r="AP25" s="1"/>
     </row>
-    <row r="26" spans="1:42" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:42" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
-      <c r="B26" s="33"/>
-      <c r="C26" s="13" t="s">
+      <c r="B26" s="24"/>
+      <c r="C26" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="15"/>
-      <c r="H26" s="16"/>
-      <c r="I26" s="16"/>
-      <c r="J26" s="16"/>
-      <c r="K26" s="15"/>
-      <c r="L26" s="15"/>
-      <c r="M26" s="15"/>
-      <c r="N26" s="15"/>
-      <c r="O26" s="15"/>
-      <c r="P26" s="15"/>
-      <c r="Q26" s="15"/>
-      <c r="R26" s="15"/>
-      <c r="S26" s="17"/>
-      <c r="T26" s="17"/>
-      <c r="U26" s="17"/>
-      <c r="V26" s="17"/>
-      <c r="W26" s="17"/>
-      <c r="X26" s="17"/>
-      <c r="Y26" s="17"/>
-      <c r="Z26" s="17"/>
-      <c r="AA26" s="17"/>
-      <c r="AB26" s="17"/>
-      <c r="AC26" s="17"/>
-      <c r="AD26" s="17"/>
-      <c r="AE26" s="17"/>
-      <c r="AF26" s="17"/>
-      <c r="AG26" s="17"/>
-      <c r="AH26" s="17"/>
-      <c r="AI26" s="17"/>
+      <c r="D26" s="80"/>
+      <c r="E26" s="80"/>
+      <c r="F26" s="80"/>
+      <c r="G26" s="78"/>
+      <c r="H26" s="79"/>
+      <c r="I26" s="79"/>
+      <c r="J26" s="79"/>
+      <c r="K26" s="78"/>
+      <c r="L26" s="78"/>
+      <c r="M26" s="78"/>
+      <c r="N26" s="78"/>
+      <c r="O26" s="78"/>
+      <c r="P26" s="78"/>
+      <c r="Q26" s="78"/>
+      <c r="R26" s="78"/>
+      <c r="S26" s="80"/>
+      <c r="T26" s="80"/>
+      <c r="U26" s="80"/>
+      <c r="V26" s="80"/>
+      <c r="W26" s="80"/>
+      <c r="X26" s="80"/>
+      <c r="Y26" s="80"/>
+      <c r="Z26" s="80"/>
+      <c r="AA26" s="80"/>
+      <c r="AB26" s="80"/>
+      <c r="AC26" s="80"/>
+      <c r="AD26" s="80"/>
+      <c r="AE26" s="80"/>
+      <c r="AF26" s="80"/>
+      <c r="AG26" s="80"/>
+      <c r="AH26" s="80"/>
+      <c r="AI26" s="80"/>
       <c r="AJ26" s="1"/>
       <c r="AK26" s="1"/>
       <c r="AL26" s="1"/>
@@ -2534,46 +2544,46 @@
       <c r="AO26" s="1"/>
       <c r="AP26" s="1"/>
     </row>
-    <row r="27" spans="1:42" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:42" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
-      <c r="B27" s="66" t="s">
+      <c r="B27" s="56" t="s">
         <v>44</v>
       </c>
-      <c r="C27" s="13" t="s">
+      <c r="C27" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="D27" s="13"/>
-      <c r="E27" s="13"/>
-      <c r="F27" s="13"/>
-      <c r="G27" s="15"/>
-      <c r="H27" s="16"/>
-      <c r="I27" s="16"/>
-      <c r="J27" s="16"/>
-      <c r="K27" s="15"/>
-      <c r="L27" s="15"/>
-      <c r="M27" s="15"/>
-      <c r="N27" s="15"/>
-      <c r="O27" s="15"/>
-      <c r="P27" s="15"/>
-      <c r="Q27" s="15"/>
-      <c r="R27" s="15"/>
-      <c r="S27" s="17"/>
-      <c r="T27" s="17"/>
-      <c r="U27" s="17"/>
-      <c r="V27" s="17"/>
-      <c r="W27" s="17"/>
-      <c r="X27" s="17"/>
-      <c r="Y27" s="17"/>
-      <c r="Z27" s="17"/>
-      <c r="AA27" s="17"/>
-      <c r="AB27" s="17"/>
-      <c r="AC27" s="17"/>
-      <c r="AD27" s="17"/>
-      <c r="AE27" s="17"/>
-      <c r="AF27" s="17"/>
-      <c r="AG27" s="17"/>
-      <c r="AH27" s="17"/>
-      <c r="AI27" s="17"/>
+      <c r="D27" s="80"/>
+      <c r="E27" s="80"/>
+      <c r="F27" s="80"/>
+      <c r="G27" s="78"/>
+      <c r="H27" s="79"/>
+      <c r="I27" s="79"/>
+      <c r="J27" s="79"/>
+      <c r="K27" s="78"/>
+      <c r="L27" s="78"/>
+      <c r="M27" s="78"/>
+      <c r="N27" s="78"/>
+      <c r="O27" s="78"/>
+      <c r="P27" s="78"/>
+      <c r="Q27" s="78"/>
+      <c r="R27" s="78"/>
+      <c r="S27" s="80"/>
+      <c r="T27" s="80"/>
+      <c r="U27" s="80"/>
+      <c r="V27" s="80"/>
+      <c r="W27" s="80"/>
+      <c r="X27" s="80"/>
+      <c r="Y27" s="80"/>
+      <c r="Z27" s="80"/>
+      <c r="AA27" s="80"/>
+      <c r="AB27" s="80"/>
+      <c r="AC27" s="80"/>
+      <c r="AD27" s="80"/>
+      <c r="AE27" s="80"/>
+      <c r="AF27" s="80"/>
+      <c r="AG27" s="80"/>
+      <c r="AH27" s="80"/>
+      <c r="AI27" s="80"/>
       <c r="AJ27" s="1"/>
       <c r="AK27" s="1"/>
       <c r="AL27" s="1"/>
@@ -2582,44 +2592,44 @@
       <c r="AO27" s="1"/>
       <c r="AP27" s="1"/>
     </row>
-    <row r="28" spans="1:42" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:42" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
-      <c r="B28" s="67"/>
-      <c r="C28" s="13" t="s">
+      <c r="B28" s="57"/>
+      <c r="C28" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="15"/>
-      <c r="H28" s="16"/>
-      <c r="I28" s="16"/>
-      <c r="J28" s="16"/>
-      <c r="K28" s="15"/>
-      <c r="L28" s="15"/>
-      <c r="M28" s="15"/>
-      <c r="N28" s="15"/>
-      <c r="O28" s="15"/>
-      <c r="P28" s="15"/>
-      <c r="Q28" s="15"/>
-      <c r="R28" s="15"/>
-      <c r="S28" s="17"/>
-      <c r="T28" s="17"/>
-      <c r="U28" s="17"/>
-      <c r="V28" s="17"/>
-      <c r="W28" s="17"/>
-      <c r="X28" s="17"/>
-      <c r="Y28" s="17"/>
-      <c r="Z28" s="17"/>
-      <c r="AA28" s="17"/>
-      <c r="AB28" s="17"/>
-      <c r="AC28" s="17"/>
-      <c r="AD28" s="17"/>
-      <c r="AE28" s="17"/>
-      <c r="AF28" s="17"/>
-      <c r="AG28" s="17"/>
-      <c r="AH28" s="17"/>
-      <c r="AI28" s="15"/>
+      <c r="D28" s="80"/>
+      <c r="E28" s="80"/>
+      <c r="F28" s="80"/>
+      <c r="G28" s="78"/>
+      <c r="H28" s="79"/>
+      <c r="I28" s="79"/>
+      <c r="J28" s="79"/>
+      <c r="K28" s="78"/>
+      <c r="L28" s="78"/>
+      <c r="M28" s="78"/>
+      <c r="N28" s="78"/>
+      <c r="O28" s="78"/>
+      <c r="P28" s="78"/>
+      <c r="Q28" s="78"/>
+      <c r="R28" s="78"/>
+      <c r="S28" s="80"/>
+      <c r="T28" s="80"/>
+      <c r="U28" s="80"/>
+      <c r="V28" s="80"/>
+      <c r="W28" s="80"/>
+      <c r="X28" s="80"/>
+      <c r="Y28" s="80"/>
+      <c r="Z28" s="80"/>
+      <c r="AA28" s="80"/>
+      <c r="AB28" s="80"/>
+      <c r="AC28" s="80"/>
+      <c r="AD28" s="80"/>
+      <c r="AE28" s="80"/>
+      <c r="AF28" s="80"/>
+      <c r="AG28" s="80"/>
+      <c r="AH28" s="80"/>
+      <c r="AI28" s="78"/>
       <c r="AJ28" s="1"/>
       <c r="AK28" s="1"/>
       <c r="AL28" s="1"/>
@@ -2628,139 +2638,139 @@
       <c r="AO28" s="1"/>
       <c r="AP28" s="1"/>
     </row>
-    <row r="29" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
-      <c r="B29" s="53" t="s">
+      <c r="B29" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="C29" s="13" t="s">
+      <c r="C29" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="D29" s="13">
+      <c r="D29" s="80">
         <f>SUM(D17,D19,D21,D23,D25,D27)</f>
         <v>0</v>
       </c>
-      <c r="E29" s="13">
+      <c r="E29" s="80">
         <f t="shared" ref="E29:AI29" si="0">SUM(E17,E19,E21,E23,E25,E27)</f>
         <v>0</v>
       </c>
-      <c r="F29" s="13">
+      <c r="F29" s="80">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G29" s="13">
+      <c r="G29" s="80">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H29" s="13">
+      <c r="H29" s="80">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I29" s="13">
+      <c r="I29" s="80">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J29" s="13">
+      <c r="J29" s="80">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K29" s="13">
+      <c r="K29" s="80">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L29" s="13">
+      <c r="L29" s="80">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M29" s="13">
+      <c r="M29" s="80">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="N29" s="13">
+      <c r="N29" s="80">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="O29" s="13">
+      <c r="O29" s="80">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="P29" s="13">
+      <c r="P29" s="80">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Q29" s="13">
+      <c r="Q29" s="80">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="R29" s="13">
+      <c r="R29" s="80">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="S29" s="13">
+      <c r="S29" s="80">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T29" s="13">
+      <c r="T29" s="80">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="U29" s="13">
+      <c r="U29" s="80">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="V29" s="13">
+      <c r="V29" s="80">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="W29" s="13">
+      <c r="W29" s="80">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="X29" s="13">
+      <c r="X29" s="80">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Y29" s="13">
+      <c r="Y29" s="80">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Z29" s="13">
+      <c r="Z29" s="80">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AA29" s="13">
+      <c r="AA29" s="80">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AB29" s="13">
+      <c r="AB29" s="80">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AC29" s="13">
+      <c r="AC29" s="80">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AD29" s="13">
+      <c r="AD29" s="80">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AE29" s="13">
+      <c r="AE29" s="80">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AF29" s="13">
+      <c r="AF29" s="80">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AG29" s="13">
+      <c r="AG29" s="80">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AH29" s="13">
+      <c r="AH29" s="80">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AI29" s="13">
+      <c r="AI29" s="80">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2772,137 +2782,137 @@
       <c r="AO29" s="1"/>
       <c r="AP29" s="1"/>
     </row>
-    <row r="30" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
-      <c r="B30" s="33"/>
-      <c r="C30" s="13" t="s">
+      <c r="B30" s="24"/>
+      <c r="C30" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="D30" s="13">
+      <c r="D30" s="80">
         <f>SUM(D18,D20,D22,D24,D26,D28)</f>
         <v>0</v>
       </c>
-      <c r="E30" s="13">
+      <c r="E30" s="80">
         <f t="shared" ref="E30:AI30" si="1">SUM(E18,E20,E22,E24,E26,E28)</f>
         <v>0</v>
       </c>
-      <c r="F30" s="13">
+      <c r="F30" s="80">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G30" s="13">
+      <c r="G30" s="80">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H30" s="13">
+      <c r="H30" s="80">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I30" s="13">
+      <c r="I30" s="80">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J30" s="13">
+      <c r="J30" s="80">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K30" s="13">
+      <c r="K30" s="80">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L30" s="13">
+      <c r="L30" s="80">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M30" s="13">
+      <c r="M30" s="80">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="N30" s="13">
+      <c r="N30" s="80">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O30" s="13">
+      <c r="O30" s="80">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="P30" s="13">
+      <c r="P30" s="80">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Q30" s="13">
+      <c r="Q30" s="80">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="R30" s="13">
+      <c r="R30" s="80">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="S30" s="13">
+      <c r="S30" s="80">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T30" s="13">
+      <c r="T30" s="80">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="U30" s="13">
+      <c r="U30" s="80">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="V30" s="13">
+      <c r="V30" s="80">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="W30" s="13">
+      <c r="W30" s="80">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="X30" s="13">
+      <c r="X30" s="80">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Y30" s="13">
+      <c r="Y30" s="80">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Z30" s="13">
+      <c r="Z30" s="80">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AA30" s="13">
+      <c r="AA30" s="80">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AB30" s="13">
+      <c r="AB30" s="80">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AC30" s="13">
+      <c r="AC30" s="80">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AD30" s="13">
+      <c r="AD30" s="80">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AE30" s="13">
+      <c r="AE30" s="80">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AF30" s="13">
+      <c r="AF30" s="80">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AG30" s="13">
+      <c r="AG30" s="80">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AH30" s="13">
+      <c r="AH30" s="80">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AI30" s="13">
+      <c r="AI30" s="80">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2914,7 +2924,7 @@
       <c r="AO30" s="1"/>
       <c r="AP30" s="1"/>
     </row>
-    <row r="31" spans="1:42" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:42" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -2956,25 +2966,25 @@
       <c r="AM31" s="1"/>
       <c r="AN31" s="1"/>
     </row>
-    <row r="32" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
-      <c r="B32" s="62" t="s">
+      <c r="B32" s="29" t="s">
         <v>31</v>
       </c>
       <c r="C32" s="30"/>
-      <c r="D32" s="19"/>
-      <c r="E32" s="19"/>
-      <c r="F32" s="19"/>
-      <c r="G32" s="19"/>
-      <c r="H32" s="19"/>
-      <c r="I32" s="19"/>
-      <c r="J32" s="19"/>
-      <c r="K32" s="19"/>
-      <c r="L32" s="19"/>
-      <c r="M32" s="19"/>
-      <c r="N32" s="19"/>
-      <c r="O32" s="19"/>
-      <c r="P32" s="19"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="13"/>
+      <c r="F32" s="13"/>
+      <c r="G32" s="13"/>
+      <c r="H32" s="13"/>
+      <c r="I32" s="13"/>
+      <c r="J32" s="13"/>
+      <c r="K32" s="13"/>
+      <c r="L32" s="13"/>
+      <c r="M32" s="13"/>
+      <c r="N32" s="13"/>
+      <c r="O32" s="13"/>
+      <c r="P32" s="13"/>
       <c r="Q32" s="1"/>
       <c r="R32" s="1"/>
       <c r="S32" s="1"/>
@@ -3000,25 +3010,25 @@
       <c r="AM32" s="1"/>
       <c r="AN32" s="1"/>
     </row>
-    <row r="33" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
-      <c r="B33" s="62" t="s">
+      <c r="B33" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="C33" s="41"/>
-      <c r="D33" s="41"/>
+      <c r="C33" s="47"/>
+      <c r="D33" s="47"/>
       <c r="E33" s="30"/>
-      <c r="F33" s="19"/>
-      <c r="G33" s="19"/>
-      <c r="H33" s="19"/>
-      <c r="I33" s="19"/>
-      <c r="J33" s="19"/>
-      <c r="K33" s="19"/>
-      <c r="L33" s="19"/>
-      <c r="M33" s="19"/>
-      <c r="N33" s="19"/>
-      <c r="O33" s="19"/>
-      <c r="P33" s="19"/>
+      <c r="F33" s="13"/>
+      <c r="G33" s="13"/>
+      <c r="H33" s="13"/>
+      <c r="I33" s="13"/>
+      <c r="J33" s="13"/>
+      <c r="K33" s="13"/>
+      <c r="L33" s="13"/>
+      <c r="M33" s="13"/>
+      <c r="N33" s="13"/>
+      <c r="O33" s="13"/>
+      <c r="P33" s="13"/>
       <c r="Q33" s="1"/>
       <c r="R33" s="1"/>
       <c r="S33" s="1"/>
@@ -3044,23 +3054,23 @@
       <c r="AM33" s="1"/>
       <c r="AN33" s="1"/>
     </row>
-    <row r="34" spans="1:40" ht="4.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:40" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
-      <c r="C34" s="20"/>
-      <c r="D34" s="20"/>
-      <c r="E34" s="19"/>
-      <c r="F34" s="19"/>
-      <c r="G34" s="19"/>
-      <c r="H34" s="19"/>
-      <c r="I34" s="19"/>
-      <c r="J34" s="19"/>
-      <c r="K34" s="19"/>
-      <c r="L34" s="19"/>
-      <c r="M34" s="19"/>
-      <c r="N34" s="19"/>
-      <c r="O34" s="19"/>
-      <c r="P34" s="19"/>
+      <c r="C34" s="14"/>
+      <c r="D34" s="14"/>
+      <c r="E34" s="13"/>
+      <c r="F34" s="13"/>
+      <c r="G34" s="13"/>
+      <c r="H34" s="13"/>
+      <c r="I34" s="13"/>
+      <c r="J34" s="13"/>
+      <c r="K34" s="13"/>
+      <c r="L34" s="13"/>
+      <c r="M34" s="13"/>
+      <c r="N34" s="13"/>
+      <c r="O34" s="13"/>
+      <c r="P34" s="13"/>
       <c r="Q34" s="1"/>
       <c r="R34" s="1"/>
       <c r="S34" s="1"/>
@@ -3086,7 +3096,7 @@
       <c r="AM34" s="1"/>
       <c r="AN34" s="1"/>
     </row>
-    <row r="35" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -3128,7 +3138,7 @@
       <c r="AM35" s="1"/>
       <c r="AN35" s="1"/>
     </row>
-    <row r="36" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -3170,7 +3180,7 @@
       <c r="AM36" s="1"/>
       <c r="AN36" s="1"/>
     </row>
-    <row r="37" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -3212,7 +3222,7 @@
       <c r="AM37" s="1"/>
       <c r="AN37" s="1"/>
     </row>
-    <row r="38" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -3254,7 +3264,7 @@
       <c r="AM38" s="1"/>
       <c r="AN38" s="1"/>
     </row>
-    <row r="39" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -3296,7 +3306,7 @@
       <c r="AM39" s="1"/>
       <c r="AN39" s="1"/>
     </row>
-    <row r="40" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -3338,7 +3348,7 @@
       <c r="AM40" s="1"/>
       <c r="AN40" s="1"/>
     </row>
-    <row r="41" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -3380,7 +3390,7 @@
       <c r="AM41" s="1"/>
       <c r="AN41" s="1"/>
     </row>
-    <row r="42" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -3422,7 +3432,7 @@
       <c r="AM42" s="1"/>
       <c r="AN42" s="1"/>
     </row>
-    <row r="43" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -3464,7 +3474,7 @@
       <c r="AM43" s="1"/>
       <c r="AN43" s="1"/>
     </row>
-    <row r="44" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -3506,7 +3516,7 @@
       <c r="AM44" s="1"/>
       <c r="AN44" s="1"/>
     </row>
-    <row r="45" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -3548,7 +3558,7 @@
       <c r="AM45" s="1"/>
       <c r="AN45" s="1"/>
     </row>
-    <row r="46" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
@@ -3590,7 +3600,7 @@
       <c r="AM46" s="1"/>
       <c r="AN46" s="1"/>
     </row>
-    <row r="47" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -3632,7 +3642,7 @@
       <c r="AM47" s="1"/>
       <c r="AN47" s="1"/>
     </row>
-    <row r="48" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -3674,7 +3684,7 @@
       <c r="AM48" s="1"/>
       <c r="AN48" s="1"/>
     </row>
-    <row r="49" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -3716,7 +3726,7 @@
       <c r="AM49" s="1"/>
       <c r="AN49" s="1"/>
     </row>
-    <row r="50" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -3758,7 +3768,7 @@
       <c r="AM50" s="1"/>
       <c r="AN50" s="1"/>
     </row>
-    <row r="51" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -3800,7 +3810,7 @@
       <c r="AM51" s="1"/>
       <c r="AN51" s="1"/>
     </row>
-    <row r="52" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -3842,7 +3852,7 @@
       <c r="AM52" s="1"/>
       <c r="AN52" s="1"/>
     </row>
-    <row r="53" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -3884,7 +3894,7 @@
       <c r="AM53" s="1"/>
       <c r="AN53" s="1"/>
     </row>
-    <row r="54" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
@@ -3926,7 +3936,7 @@
       <c r="AM54" s="1"/>
       <c r="AN54" s="1"/>
     </row>
-    <row r="55" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
@@ -3968,7 +3978,7 @@
       <c r="AM55" s="1"/>
       <c r="AN55" s="1"/>
     </row>
-    <row r="56" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
@@ -4010,7 +4020,7 @@
       <c r="AM56" s="1"/>
       <c r="AN56" s="1"/>
     </row>
-    <row r="57" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
@@ -4052,7 +4062,7 @@
       <c r="AM57" s="1"/>
       <c r="AN57" s="1"/>
     </row>
-    <row r="58" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -4094,7 +4104,7 @@
       <c r="AM58" s="1"/>
       <c r="AN58" s="1"/>
     </row>
-    <row r="59" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
@@ -4136,7 +4146,7 @@
       <c r="AM59" s="1"/>
       <c r="AN59" s="1"/>
     </row>
-    <row r="60" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -4178,7 +4188,7 @@
       <c r="AM60" s="1"/>
       <c r="AN60" s="1"/>
     </row>
-    <row r="61" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
@@ -4220,7 +4230,7 @@
       <c r="AM61" s="1"/>
       <c r="AN61" s="1"/>
     </row>
-    <row r="62" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
@@ -4262,7 +4272,7 @@
       <c r="AM62" s="1"/>
       <c r="AN62" s="1"/>
     </row>
-    <row r="63" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
@@ -4304,7 +4314,7 @@
       <c r="AM63" s="1"/>
       <c r="AN63" s="1"/>
     </row>
-    <row r="64" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
@@ -4346,7 +4356,7 @@
       <c r="AM64" s="1"/>
       <c r="AN64" s="1"/>
     </row>
-    <row r="65" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
@@ -4388,7 +4398,7 @@
       <c r="AM65" s="1"/>
       <c r="AN65" s="1"/>
     </row>
-    <row r="66" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
@@ -4430,7 +4440,7 @@
       <c r="AM66" s="1"/>
       <c r="AN66" s="1"/>
     </row>
-    <row r="67" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
@@ -4472,7 +4482,7 @@
       <c r="AM67" s="1"/>
       <c r="AN67" s="1"/>
     </row>
-    <row r="68" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
@@ -4514,7 +4524,7 @@
       <c r="AM68" s="1"/>
       <c r="AN68" s="1"/>
     </row>
-    <row r="69" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
@@ -4556,7 +4566,7 @@
       <c r="AM69" s="1"/>
       <c r="AN69" s="1"/>
     </row>
-    <row r="70" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
@@ -4598,7 +4608,7 @@
       <c r="AM70" s="1"/>
       <c r="AN70" s="1"/>
     </row>
-    <row r="71" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
@@ -4640,7 +4650,7 @@
       <c r="AM71" s="1"/>
       <c r="AN71" s="1"/>
     </row>
-    <row r="72" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="1"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
@@ -4682,7 +4692,7 @@
       <c r="AM72" s="1"/>
       <c r="AN72" s="1"/>
     </row>
-    <row r="73" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
@@ -4724,7 +4734,7 @@
       <c r="AM73" s="1"/>
       <c r="AN73" s="1"/>
     </row>
-    <row r="74" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
@@ -4766,7 +4776,7 @@
       <c r="AM74" s="1"/>
       <c r="AN74" s="1"/>
     </row>
-    <row r="75" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
@@ -4808,7 +4818,7 @@
       <c r="AM75" s="1"/>
       <c r="AN75" s="1"/>
     </row>
-    <row r="76" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="1"/>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
@@ -4850,7 +4860,7 @@
       <c r="AM76" s="1"/>
       <c r="AN76" s="1"/>
     </row>
-    <row r="77" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
@@ -4892,7 +4902,7 @@
       <c r="AM77" s="1"/>
       <c r="AN77" s="1"/>
     </row>
-    <row r="78" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
@@ -4934,7 +4944,7 @@
       <c r="AM78" s="1"/>
       <c r="AN78" s="1"/>
     </row>
-    <row r="79" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
@@ -4976,7 +4986,7 @@
       <c r="AM79" s="1"/>
       <c r="AN79" s="1"/>
     </row>
-    <row r="80" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
@@ -5018,7 +5028,7 @@
       <c r="AM80" s="1"/>
       <c r="AN80" s="1"/>
     </row>
-    <row r="81" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="1"/>
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
@@ -5060,7 +5070,7 @@
       <c r="AM81" s="1"/>
       <c r="AN81" s="1"/>
     </row>
-    <row r="82" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
@@ -5102,7 +5112,7 @@
       <c r="AM82" s="1"/>
       <c r="AN82" s="1"/>
     </row>
-    <row r="83" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="1"/>
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
@@ -5144,7 +5154,7 @@
       <c r="AM83" s="1"/>
       <c r="AN83" s="1"/>
     </row>
-    <row r="84" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="1"/>
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
@@ -5186,7 +5196,7 @@
       <c r="AM84" s="1"/>
       <c r="AN84" s="1"/>
     </row>
-    <row r="85" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="1"/>
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
@@ -5228,7 +5238,7 @@
       <c r="AM85" s="1"/>
       <c r="AN85" s="1"/>
     </row>
-    <row r="86" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="1"/>
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
@@ -5270,7 +5280,7 @@
       <c r="AM86" s="1"/>
       <c r="AN86" s="1"/>
     </row>
-    <row r="87" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="1"/>
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
@@ -5312,7 +5322,7 @@
       <c r="AM87" s="1"/>
       <c r="AN87" s="1"/>
     </row>
-    <row r="88" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="1"/>
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
@@ -5354,7 +5364,7 @@
       <c r="AM88" s="1"/>
       <c r="AN88" s="1"/>
     </row>
-    <row r="89" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="1"/>
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
@@ -5396,7 +5406,7 @@
       <c r="AM89" s="1"/>
       <c r="AN89" s="1"/>
     </row>
-    <row r="90" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="1"/>
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
@@ -5438,7 +5448,7 @@
       <c r="AM90" s="1"/>
       <c r="AN90" s="1"/>
     </row>
-    <row r="91" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="1"/>
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
@@ -5480,7 +5490,7 @@
       <c r="AM91" s="1"/>
       <c r="AN91" s="1"/>
     </row>
-    <row r="92" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="1"/>
       <c r="B92" s="1"/>
       <c r="C92" s="1"/>
@@ -5522,7 +5532,7 @@
       <c r="AM92" s="1"/>
       <c r="AN92" s="1"/>
     </row>
-    <row r="93" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="1"/>
       <c r="B93" s="1"/>
       <c r="C93" s="1"/>
@@ -5564,7 +5574,7 @@
       <c r="AM93" s="1"/>
       <c r="AN93" s="1"/>
     </row>
-    <row r="94" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="1"/>
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
@@ -5606,7 +5616,7 @@
       <c r="AM94" s="1"/>
       <c r="AN94" s="1"/>
     </row>
-    <row r="95" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="1"/>
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
@@ -5648,7 +5658,7 @@
       <c r="AM95" s="1"/>
       <c r="AN95" s="1"/>
     </row>
-    <row r="96" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="1"/>
       <c r="B96" s="1"/>
       <c r="C96" s="1"/>
@@ -5690,7 +5700,7 @@
       <c r="AM96" s="1"/>
       <c r="AN96" s="1"/>
     </row>
-    <row r="97" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="1"/>
       <c r="B97" s="1"/>
       <c r="C97" s="1"/>
@@ -5732,7 +5742,7 @@
       <c r="AM97" s="1"/>
       <c r="AN97" s="1"/>
     </row>
-    <row r="98" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="1"/>
       <c r="B98" s="1"/>
       <c r="C98" s="1"/>
@@ -5774,7 +5784,7 @@
       <c r="AM98" s="1"/>
       <c r="AN98" s="1"/>
     </row>
-    <row r="99" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="1"/>
       <c r="B99" s="1"/>
       <c r="C99" s="1"/>
@@ -5816,7 +5826,7 @@
       <c r="AM99" s="1"/>
       <c r="AN99" s="1"/>
     </row>
-    <row r="100" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="1"/>
       <c r="B100" s="1"/>
       <c r="C100" s="1"/>
@@ -5858,7 +5868,7 @@
       <c r="AM100" s="1"/>
       <c r="AN100" s="1"/>
     </row>
-    <row r="101" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="1"/>
       <c r="B101" s="1"/>
       <c r="C101" s="1"/>
@@ -5900,7 +5910,7 @@
       <c r="AM101" s="1"/>
       <c r="AN101" s="1"/>
     </row>
-    <row r="102" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B102" s="1"/>
       <c r="C102" s="1"/>
       <c r="D102" s="1"/>
@@ -5934,7 +5944,7 @@
       <c r="AF102" s="1"/>
       <c r="AG102" s="1"/>
     </row>
-    <row r="103" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B103" s="1"/>
       <c r="C103" s="1"/>
       <c r="D103" s="1"/>
@@ -5970,16 +5980,32 @@
     </row>
   </sheetData>
   <mergeCells count="52">
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="AE13:AF13"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="D11:D15"/>
-    <mergeCell ref="E11:G12"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="AE14:AE15"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="I13:I15"/>
+    <mergeCell ref="J13:J15"/>
+    <mergeCell ref="H11:J12"/>
+    <mergeCell ref="C6:AG6"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="S12:U12"/>
+    <mergeCell ref="B11:B15"/>
+    <mergeCell ref="AG11:AG15"/>
+    <mergeCell ref="C11:C15"/>
+    <mergeCell ref="AI11:AI15"/>
+    <mergeCell ref="AD11:AF12"/>
+    <mergeCell ref="U13:U15"/>
+    <mergeCell ref="V13:V15"/>
+    <mergeCell ref="G13:G15"/>
+    <mergeCell ref="H13:H15"/>
+    <mergeCell ref="AH11:AH15"/>
+    <mergeCell ref="AF14:AF15"/>
+    <mergeCell ref="L14:N14"/>
+    <mergeCell ref="X13:X15"/>
+    <mergeCell ref="Y13:Y15"/>
+    <mergeCell ref="K12:R12"/>
+    <mergeCell ref="V12:AB12"/>
+    <mergeCell ref="AC12:AC15"/>
+    <mergeCell ref="K11:R11"/>
+    <mergeCell ref="S11:AC11"/>
     <mergeCell ref="B33:E33"/>
     <mergeCell ref="S13:S15"/>
     <mergeCell ref="K13:R13"/>
@@ -5996,32 +6022,16 @@
     <mergeCell ref="B29:B30"/>
     <mergeCell ref="K14:K15"/>
     <mergeCell ref="B19:B20"/>
-    <mergeCell ref="AI11:AI15"/>
-    <mergeCell ref="AD11:AF12"/>
-    <mergeCell ref="U13:U15"/>
-    <mergeCell ref="V13:V15"/>
-    <mergeCell ref="G13:G15"/>
-    <mergeCell ref="H13:H15"/>
-    <mergeCell ref="AH11:AH15"/>
-    <mergeCell ref="AF14:AF15"/>
-    <mergeCell ref="L14:N14"/>
-    <mergeCell ref="X13:X15"/>
-    <mergeCell ref="Y13:Y15"/>
-    <mergeCell ref="K12:R12"/>
-    <mergeCell ref="V12:AB12"/>
-    <mergeCell ref="AC12:AC15"/>
-    <mergeCell ref="K11:R11"/>
-    <mergeCell ref="S11:AC11"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="I13:I15"/>
-    <mergeCell ref="J13:J15"/>
-    <mergeCell ref="H11:J12"/>
-    <mergeCell ref="C6:AG6"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="S12:U12"/>
-    <mergeCell ref="B11:B15"/>
-    <mergeCell ref="AG11:AG15"/>
-    <mergeCell ref="C11:C15"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="AE13:AF13"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="D11:D15"/>
+    <mergeCell ref="E11:G12"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="AE14:AE15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" scale="49" fitToHeight="0" orientation="landscape" r:id="rId1"/>

</xml_diff>